<commit_message>
📊 Horarios actualizados Línea 141 - 130
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:57:13</t>
+          <t>Última actualización: 06:17:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -562,21 +562,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>06:17</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -592,16 +592,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:34</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -612,21 +612,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:32</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -642,16 +642,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:41</t>
+          <t>06:34</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -667,16 +667,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -692,16 +692,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -717,16 +717,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -742,16 +742,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -762,21 +762,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -792,16 +792,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -817,16 +817,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -842,16 +842,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,23 +862,248 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>07:29</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>92</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>98</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>79</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>100</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>07:55</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D26" t="n">
         <v>118</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>103</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>104</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>114</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>116</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -895,7 +1120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,14 +1138,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:57:13</t>
+          <t>Última actualización: 06:17:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -979,12 +1204,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:17</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -993,7 +1218,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1009,18 +1234,68 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>60</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>58</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>07:16</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D10" t="n">
         <v>79</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1055,7 +1330,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:57:13</t>
+          <t>Última actualización: 06:17:28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 131
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:17:28</t>
+          <t>Última actualización: 06:35:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -662,21 +662,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:35:22</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06:39</t>
+          <t>06:35</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -692,16 +692,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06:41</t>
+          <t>06:39</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -717,16 +717,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:41</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -742,16 +742,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -762,21 +762,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -787,12 +787,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -817,16 +817,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -842,16 +842,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -872,11 +872,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -887,21 +887,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -917,16 +917,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,21 +937,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,12 +962,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -976,7 +976,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -992,16 +992,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1012,21 +1012,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:35:22</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:44</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,21 +1037,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1067,16 +1067,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1092,18 +1092,143 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>08:01</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>104</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>91</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>114</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>08:13</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="D33" t="n">
         <v>116</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>114</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>114</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1120,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1138,14 +1263,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:17:28</t>
+          <t>Última actualización: 06:35:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1296,6 +1421,31 @@
         <v>79</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>69</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1330,7 +1480,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:17:28</t>
+          <t>Última actualización: 06:35:22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 132
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:35:22</t>
+          <t>Última actualización: 06:46:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -737,12 +737,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -767,16 +767,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -787,21 +787,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -812,12 +812,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -842,16 +842,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>07:19</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -867,16 +867,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -887,12 +887,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:20</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -917,16 +917,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,21 +937,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -962,21 +962,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -992,16 +992,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1012,21 +1012,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1042,16 +1042,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1062,21 +1062,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1087,21 +1087,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:35:22</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>07:44</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1112,21 +1112,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1162,21 +1162,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>08:13</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,21 +1187,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1217,18 +1217,168 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>08:06</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>91</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>08:11</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>114</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>08:13</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>116</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>08:29</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>114</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D39" t="n">
         <v>114</v>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>115</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>117</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1245,7 +1395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1263,14 +1413,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:35:22</t>
+          <t>Última actualización: 06:46:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -1354,12 +1504,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>06:56</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1368,7 +1518,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1379,21 +1529,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:57</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1404,12 +1554,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1418,7 +1568,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1429,23 +1579,98 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>57</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>06:35:22</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>07:44</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D13" t="n">
         <v>69</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1462,7 +1687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1480,14 +1705,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:35:22</t>
+          <t>Última actualización: 06:46:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -1521,23 +1746,73 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>07:42</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>56</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>07:43</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>106</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>109</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 133
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:46:50</t>
+          <t>Última actualización: 06:54:04</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -962,21 +962,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>07:29</t>
+          <t>07:22</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -992,16 +992,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>07:35</t>
+          <t>07:29</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1012,21 +1012,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>07:36</t>
+          <t>07:35</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,12 +1037,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1062,21 +1062,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1087,12 +1087,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1112,21 +1112,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:35:22</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>07:55</t>
+          <t>07:44</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1137,21 +1137,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1172,11 +1172,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,12 +1187,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>08:01</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1212,21 +1212,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>08:01</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,21 +1237,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:35:22</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>08:11</t>
+          <t>08:06</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1262,21 +1262,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>08:13</t>
+          <t>08:07</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1287,17 +1287,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1312,21 +1312,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>08:29</t>
+          <t>08:13</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1337,21 +1337,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:35:22</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>08:41</t>
+          <t>08:29</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1362,23 +1362,98 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08:29</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>114</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>06:46:50</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>08:41</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>115</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>08:43</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D43" t="n">
         <v>117</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>110</v>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1395,7 +1470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1413,14 +1488,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:46:50</t>
+          <t>Última actualización: 06:54:04</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -1671,6 +1746,31 @@
         <v>117</v>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>110</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1687,7 +1787,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,14 +1805,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:46:50</t>
+          <t>Última actualización: 06:54:04</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -1815,6 +1915,56 @@
       <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>08:36</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>102</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>117</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 134
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:54:04</t>
+          <t>Última actualización: 07:12:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -1454,6 +1454,81 @@
         <v>110</v>
       </c>
       <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>08:51</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>99</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>101</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>105</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1470,7 +1545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1488,14 +1563,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:54:04</t>
+          <t>Última actualización: 07:12:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -1771,6 +1846,56 @@
         <v>110</v>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>101</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>105</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1787,7 +1912,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1805,14 +1930,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:54:04</t>
+          <t>Última actualización: 07:12:46</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1946,23 +2071,48 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>08:50</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>98</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>06:54:04</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>08:51</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>117</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 135
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:12:46</t>
+          <t>Última actualización: 07:38:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1529,6 +1529,156 @@
         <v>105</v>
       </c>
       <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>80</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>09:06</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>88</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>98</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>09:17</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>99</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>09:18</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>100</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>09:29</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>111</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1545,7 +1695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1563,14 +1713,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:12:46</t>
+          <t>Última actualización: 07:38:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -1896,6 +2046,31 @@
         <v>105</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>80</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1930,7 +2105,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:12:46</t>
+          <t>Última actualización: 07:38:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 136
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:38:39</t>
+          <t>Última actualización: 07:50:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
     </row>
@@ -1462,12 +1462,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:49</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1476,7 +1476,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1492,16 +1492,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1517,16 +1517,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1537,12 +1537,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1567,16 +1567,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1592,16 +1592,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1617,16 +1617,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1642,16 +1642,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1667,18 +1667,118 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>09:18</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>100</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>09:29</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="D54" t="n">
         <v>111</v>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>109</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>111</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>113</v>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1713,7 +1813,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:38:39</t>
+          <t>Última actualización: 07:50:33</t>
         </is>
       </c>
     </row>
@@ -2087,7 +2187,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2105,14 +2205,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:38:39</t>
+          <t>Última actualización: 07:50:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -2290,6 +2390,31 @@
       <c r="E11" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>91</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 137
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:50:33</t>
+          <t>Última actualización: 08:10:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 52</t>
+          <t>Total filas: 61</t>
         </is>
       </c>
     </row>
@@ -1537,21 +1537,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,12 +1562,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1576,7 +1576,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1592,16 +1592,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,21 +1612,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1642,16 +1642,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1667,16 +1667,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1692,16 +1692,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,21 +1712,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,23 +1762,248 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>09:29</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>111</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>09:31</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>81</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>09:36</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>86</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
           <t>07:50:33</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>09:39</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>109</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>111</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>92</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
         <is>
           <t>09:43</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D57" t="n">
+      <c r="D63" t="n">
         <v>113</v>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>103</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>109</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>10:06</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>116</v>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1795,7 +2020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1813,14 +2038,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:50:33</t>
+          <t>Última actualización: 08:10:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -2129,21 +2354,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2154,23 +2379,73 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>105</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>07:38:39</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>08:58</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D19" t="n">
         <v>80</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>109</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2205,7 +2480,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:50:33</t>
+          <t>Última actualización: 08:10:18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 138
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:10:18</t>
+          <t>Última actualización: 08:27:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 61</t>
+          <t>Total filas: 65</t>
         </is>
       </c>
     </row>
@@ -1512,21 +1512,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1537,12 +1537,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,21 +1562,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,12 +1587,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1601,7 +1601,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,21 +1612,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1637,21 +1637,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1667,16 +1667,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1692,16 +1692,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,21 +1712,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1742,16 +1742,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1787,21 +1787,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>09:36</t>
+          <t>09:29</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1837,21 +1837,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1862,21 +1862,21 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:36</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1887,21 +1887,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,21 +1912,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1937,21 +1937,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1967,16 +1967,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,23 +1987,123 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>113</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>08:10:18</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>09:53</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>103</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>109</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>10:06</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D66" t="n">
+      <c r="D69" t="n">
         <v>116</v>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>08:27:16</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>106</v>
+      </c>
+      <c r="E70" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2038,7 +2138,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:10:18</t>
+          <t>Última actualización: 08:27:16</t>
         </is>
       </c>
     </row>
@@ -2462,7 +2562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2480,14 +2580,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:10:18</t>
+          <t>Última actualización: 08:27:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -2690,6 +2790,31 @@
       <c r="E12" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08:27:16</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>106</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 139
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:27:16</t>
+          <t>Última actualización: 08:37:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 65</t>
+          <t>Total filas: 67</t>
         </is>
       </c>
     </row>
@@ -1712,7 +1712,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1722,11 +1722,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2062,12 +2062,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>10:06</t>
+          <t>10:05</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2076,7 +2076,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,23 +2087,73 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>10:06</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>116</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>08:27:16</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B71" t="inlineStr">
         <is>
           <t>10:13</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>17X38_ROMERO</t>
         </is>
       </c>
-      <c r="D70" t="n">
+      <c r="D71" t="n">
         <v>106</v>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>08:37:25</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>112</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2138,7 +2188,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:27:16</t>
+          <t>Última actualización: 08:37:25</t>
         </is>
       </c>
     </row>
@@ -2562,7 +2612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2580,14 +2630,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:27:16</t>
+          <t>Última actualización: 08:37:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 10</t>
         </is>
       </c>
     </row>
@@ -2721,37 +2771,37 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>08:50</t>
+          <t>08:37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>06:54:04</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2760,7 +2810,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2771,50 +2821,100 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>07:50:33</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>91</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>08:27:16</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>10:13</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D14" t="n">
         <v>106</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>08:37:25</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>113</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 140
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:37:25</t>
+          <t>Última actualización: 08:45:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 67</t>
+          <t>Total filas: 69</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1462,21 +1462,21 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>08:49</t>
+          <t>08:46</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,12 +1487,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>08:51</t>
+          <t>08:49</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1501,7 +1501,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1512,12 +1512,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>08:52</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1537,21 +1537,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,12 +1562,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1576,7 +1576,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,21 +1587,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,12 +1612,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1626,7 +1626,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1637,21 +1637,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>08:58</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,21 +1662,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>09:06</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1692,16 +1692,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1717,16 +1717,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>09:18</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>09:18</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1837,21 +1837,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>09:31</t>
+          <t>09:29</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1867,16 +1867,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>09:36</t>
+          <t>09:31</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1887,21 +1887,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:36</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1937,21 +1937,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,12 +1962,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1976,7 +1976,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,21 +1987,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2042,16 +2042,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>09:59</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,12 +2087,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>10:06</t>
+          <t>10:05</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2101,7 +2101,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,21 +2112,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:06</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,23 +2137,73 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
+          <t>08:27:16</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>106</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
           <t>08:37:25</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B73" t="inlineStr">
         <is>
           <t>10:29</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D72" t="n">
+      <c r="D73" t="n">
         <v>112</v>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>08:45:36</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>119</v>
+      </c>
+      <c r="E74" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2170,7 +2220,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2188,14 +2238,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:37:25</t>
+          <t>Última actualización: 08:45:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -2479,21 +2529,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:46</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2504,12 +2554,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2518,7 +2568,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2529,21 +2579,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2554,12 +2604,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>08:57</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2568,7 +2618,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2579,23 +2629,48 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>80</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>08:10:18</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>09:59</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>109</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2612,7 +2687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2630,14 +2705,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:37:25</t>
+          <t>Última actualización: 08:45:36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 10</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -2871,12 +2946,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2885,7 +2960,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2896,23 +2971,73 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>08:27:16</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>106</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>08:37:25</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>10:30</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D16" t="n">
         <v>113</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>08:45:36</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>10:31</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>106</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 141
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:45:36</t>
+          <t>Última actualización: 08:52:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 69</t>
+          <t>Total filas: 72</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1887,12 +1887,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>09:36</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1901,7 +1901,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,21 +1912,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>09:39</t>
+          <t>09:36</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,21 +1962,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:39</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,12 +1987,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2001,7 +2001,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2037,21 +2037,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>09:53</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2067,16 +2067,16 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>09:53</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2117,16 +2117,16 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10:06</t>
+          <t>09:59</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,21 +2137,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>10:13</t>
+          <t>10:05</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2162,21 +2162,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:06</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2187,23 +2187,98 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>08:27:16</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>10:13</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>106</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>08:37:25</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>112</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
           <t>08:45:36</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B76" t="inlineStr">
         <is>
           <t>10:44</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D74" t="n">
+      <c r="D76" t="n">
         <v>119</v>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>08:52:50</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>10:46</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>15_P INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>114</v>
+      </c>
+      <c r="E77" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2215,6 +2290,498 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 08:52:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:17</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>60</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>58</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>57</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>69</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>110</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:45:36</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:46</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>101</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>44</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>105</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>80</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:52:50</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>66</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>109</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2231,14 +2798,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:45:36</t>
+          <t>Última actualización: 08:52:50</t>
         </is>
       </c>
     </row>
@@ -2279,50 +2846,50 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>07:42</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:17</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2334,195 +2901,195 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:54:04</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2534,510 +3101,143 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:46</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>10:31</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E21" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 08:45:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 12</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>07:42</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>56</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05:57:13</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>106</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>08:35</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>109</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08:36</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>102</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>08:37</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>07:12:46</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>98</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>08:51</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>117</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>07:50:33</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>09:21</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>91</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>10:12</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>87</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>08:27:16</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>10:13</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>106</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>113</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>10:31</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>106</v>
-      </c>
-      <c r="E17" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 142
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:50</t>
+          <t>Última actualización: 09:23:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 72</t>
+          <t>Total filas: 81</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2212,21 +2212,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>10:29</t>
+          <t>10:21</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,21 +2237,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>08:45:36</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:25</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,23 +2262,248 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
+          <t>08:37:25</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>112</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>10:29</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>66</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>08:45:36</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>119</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>08:52:50</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>10:46</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>15_P INDUSTRIAL</t>
         </is>
       </c>
-      <c r="D77" t="n">
+      <c r="D80" t="n">
         <v>114</v>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>10:57</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>94</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>96</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>98</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>107</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>111</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>112</v>
+      </c>
+      <c r="E86" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2313,7 +2538,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:50</t>
+          <t>Última actualización: 09:23:23</t>
         </is>
       </c>
     </row>
@@ -2805,7 +3030,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:52:50</t>
+          <t>Última actualización: 09:23:23</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 143
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:23:23</t>
+          <t>Última actualización: 10:05:51</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 81</t>
+          <t>Total filas: 93</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -2312,12 +2312,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>08:45:36</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:43</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2326,7 +2326,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,21 +2337,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:52:50</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10:46</t>
+          <t>10:44</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>15_P INDUSTRIAL</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,21 +2362,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10:57</t>
+          <t>10:46</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_P INDUSTRIAL</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2387,21 +2387,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>10:55</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:56</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2442,16 +2442,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>10:57</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>10:58</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2492,18 +2492,318 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>96</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>98</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>59</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>107</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>11:14</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>111</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>09:23:23</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
           <t>11:15</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C91" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D86" t="n">
+      <c r="D91" t="n">
         <v>112</v>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>11:28</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>83</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>85</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>86</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>96</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>100</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>107</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>113</v>
+      </c>
+      <c r="E98" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2515,6 +2815,548 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 10:05:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 19</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:17</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>60</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>58</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>57</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>69</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>110</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:45:36</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:46</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>101</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>44</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>105</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>80</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:52:50</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>66</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>109</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>85</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>96</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2531,14 +3373,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:23:23</t>
+          <t>Última actualización: 10:05:51</t>
         </is>
       </c>
     </row>
@@ -2579,50 +3421,50 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>07:42</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:17</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2634,195 +3476,195 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:54:04</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -2834,637 +3676,170 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:46</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>08:52:50</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>10:31</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 09:23:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 16</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>07:42</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>56</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05:57:13</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>106</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>08:35</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>109</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08:36</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>102</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>08:37</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>07:12:46</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>98</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
           <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>08:51</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>117</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>08:52</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>09:20</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>28</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>07:50:33</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>09:21</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>91</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>87</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:27:16</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>10:13</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>106</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>10:29</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>97</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>113</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>98</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10:31</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>106</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 144
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:05:51</t>
+          <t>Última actualización: 10:37:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 93</t>
+          <t>Total filas: 103</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>11:06</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2592,16 +2592,16 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:10</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2617,16 +2617,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:14</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>11:28</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2692,16 +2692,16 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>11:28</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2717,16 +2717,16 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2742,16 +2742,16 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2767,16 +2767,16 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2792,18 +2792,268 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>100</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>11:52</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>107</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>11:53</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>76</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
           <t>11:58</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D98" t="n">
+      <c r="D101" t="n">
         <v>113</v>
       </c>
-      <c r="E98" t="inlineStr">
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>12:05</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>88</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>93</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>93</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>12:16</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>99</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>104</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>115</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>117</v>
+      </c>
+      <c r="E108" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2820,7 +3070,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2838,14 +3088,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:05:51</t>
+          <t>Última actualización: 10:37:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -3346,6 +3596,31 @@
         <v>96</v>
       </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>104</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3380,7 +3655,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:05:51</t>
+          <t>Última actualización: 10:37:52</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 145
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:37:52</t>
+          <t>Última actualización: 10:50:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 103</t>
+          <t>Total filas: 109</t>
         </is>
       </c>
     </row>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>11:04</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,12 +2562,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>11:06</t>
+          <t>11:04</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2576,7 +2576,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>11:06</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2617,16 +2617,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:10</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2642,16 +2642,16 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:14</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>11:25</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>11:28</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2717,16 +2717,16 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:28</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,21 +2737,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2767,16 +2767,16 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2792,16 +2792,16 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2817,16 +2817,16 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2867,16 +2867,16 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2892,16 +2892,16 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2992,16 +2992,16 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3017,16 +3017,16 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3042,18 +3042,168 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
+          <t>12:10</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>93</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>12:16</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>99</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>104</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>115</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
           <t>12:34</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
+      <c r="C112" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D108" t="n">
+      <c r="D112" t="n">
         <v>117</v>
       </c>
-      <c r="E108" t="inlineStr">
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>10:50:41</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>106</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>10:50:41</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>118</v>
+      </c>
+      <c r="E114" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3088,7 +3238,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:37:52</t>
+          <t>Última actualización: 10:50:41</t>
         </is>
       </c>
     </row>
@@ -3655,7 +3805,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:37:52</t>
+          <t>Última actualización: 10:50:41</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 146
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:50:41</t>
+          <t>Última actualización: 11:11:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 109</t>
+          <t>Total filas: 117</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:11</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2667,16 +2667,16 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>11:15</t>
+          <t>11:14</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>11:25</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,21 +2712,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>11:28</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,12 +2737,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>11:29</t>
+          <t>11:28</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2751,7 +2751,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,21 +2762,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2792,16 +2792,16 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2817,16 +2817,16 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2867,16 +2867,16 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2887,21 +2887,21 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>11:54</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3067,16 +3067,16 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3092,16 +3092,16 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3117,16 +3117,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3142,16 +3142,16 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,23 +3187,223 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>104</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>71</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>12:32</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>115</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>117</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>84</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
           <t>10:50:41</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>106</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>10:50:41</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
         <is>
           <t>12:48</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr">
+      <c r="C120" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D114" t="n">
+      <c r="D120" t="n">
         <v>118</v>
       </c>
-      <c r="E114" t="inlineStr">
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>97</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>111</v>
+      </c>
+      <c r="E122" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3220,7 +3420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3238,14 +3438,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:50:41</t>
+          <t>Última actualización: 11:11:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -3729,21 +3929,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:31</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3754,23 +3954,73 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>96</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>10:37:52</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>12:21</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D26" t="n">
         <v>104</v>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>71</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3805,7 +4055,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:50:41</t>
+          <t>Última actualización: 11:11:33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 147
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:11:33</t>
+          <t>Última actualización: 11:34:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 117</t>
+          <t>Total filas: 132</t>
         </is>
       </c>
     </row>
@@ -2887,12 +2887,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:44</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -3012,12 +3012,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11:54</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3026,7 +3026,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:57</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,21 +3087,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3117,16 +3117,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3192,16 +3192,16 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3242,16 +3242,16 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,23 +3387,398 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>12:34</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>117</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
           <t>11:11:33</t>
         </is>
       </c>
-      <c r="B122" t="inlineStr">
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>84</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>61</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>10:50:41</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>106</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>62</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>12:47</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>73</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>12:47</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>73</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>12:47</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>73</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>97</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>10:50:41</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>118</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
         <is>
           <t>13:02</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr">
+      <c r="C132" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D122" t="n">
+      <c r="D132" t="n">
         <v>111</v>
       </c>
-      <c r="E122" t="inlineStr">
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>89</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>13:12</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>98</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>13:16</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>102</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>13:24</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>110</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>118</v>
+      </c>
+      <c r="E137" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3420,7 +3795,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3438,14 +3813,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:11:33</t>
+          <t>Última actualización: 11:34:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -4021,6 +4396,56 @@
         <v>71</v>
       </c>
       <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>89</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>118</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4037,7 +4462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4055,14 +4480,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:11:33</t>
+          <t>Última actualización: 11:34:59</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -4515,6 +4940,56 @@
       <c r="E22" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>13:11</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>97</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>106</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 148
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:34:59</t>
+          <t>Última actualización: 11:47:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 132</t>
+          <t>Total filas: 145</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2272,11 +2272,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:47</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>11:52</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,12 +2987,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,12 +3012,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3026,7 +3026,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3042,16 +3042,16 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>11:54</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>11:57</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,21 +3087,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,21 +3112,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:57</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,12 +3212,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3226,7 +3226,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3292,16 +3292,16 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,12 +3412,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3426,7 +3426,7 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,21 +3437,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,21 +3462,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3492,16 +3492,16 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,21 +3537,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3567,16 +3567,16 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,21 +3587,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,21 +3612,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,21 +3637,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3667,16 +3667,16 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3692,16 +3692,16 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>13:12</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3717,16 +3717,16 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>13:16</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,21 +3737,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,23 +3762,348 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>61</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>97</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>111</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
           <t>11:34:59</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>89</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>76</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>77</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>13:12</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>98</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>13:13</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>86</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>13:16</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>102</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>90</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>13:24</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>110</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>98</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
         <is>
           <t>13:32</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr">
+      <c r="C149" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D137" t="n">
+      <c r="D149" t="n">
         <v>118</v>
       </c>
-      <c r="E137" t="inlineStr">
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>106</v>
+      </c>
+      <c r="E150" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3795,7 +4120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3813,14 +4138,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:34:59</t>
+          <t>Última actualización: 11:47:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -4429,23 +4754,73 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>77</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>11:34:59</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>13:32</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D30" t="n">
         <v>118</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>106</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4462,7 +4837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4480,14 +4855,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:34:59</t>
+          <t>Última actualización: 11:47:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -4971,23 +5346,73 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>13:12</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>85</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>11:34:59</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>13:20</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D25" t="n">
         <v>106</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>94</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 149
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:47:17</t>
+          <t>Última actualización: 11:52:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 145</t>
+          <t>Total filas: 149</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1172,11 +1172,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1197,11 +1197,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3022,11 +3022,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,12 +3037,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>11:53</t>
+          <t>11:52</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3051,7 +3051,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3072,11 +3072,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,12 +3087,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>11:54</t>
+          <t>11:53</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3101,7 +3101,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3112,21 +3112,21 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>11:57</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:57</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3317,16 +3317,16 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3367,16 +3367,16 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3392,16 +3392,16 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,21 +3412,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,21 +3437,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3467,16 +3467,16 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,21 +3487,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,21 +3537,21 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,21 +3562,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,21 +3587,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3617,16 +3617,16 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,12 +3637,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3651,7 +3651,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3667,16 +3667,16 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,21 +3712,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,12 +3737,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3751,7 +3751,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,12 +3762,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3776,7 +3776,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,12 +3787,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3801,7 +3801,7 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3812,21 +3812,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3837,21 +3837,21 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,21 +3862,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3887,21 +3887,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3917,16 +3917,16 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>13:12</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3942,16 +3942,16 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3962,21 +3962,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>13:16</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3987,21 +3987,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:12</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,21 +4012,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4037,21 +4037,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:16</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4062,21 +4062,21 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4087,23 +4087,123 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>13:24</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>110</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
           <t>11:47:17</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>98</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>118</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
         <is>
           <t>13:33</t>
         </is>
       </c>
-      <c r="C150" t="inlineStr">
+      <c r="C153" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D150" t="n">
+      <c r="D153" t="n">
         <v>106</v>
       </c>
-      <c r="E150" t="inlineStr">
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>11:52:01</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>115</v>
+      </c>
+      <c r="E154" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4138,7 +4238,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:47:17</t>
+          <t>Última actualización: 11:52:01</t>
         </is>
       </c>
     </row>
@@ -4855,7 +4955,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:47:17</t>
+          <t>Última actualización: 11:52:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 150
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:52:01</t>
+          <t>Última actualización: 11:54:18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 149</t>
+          <t>Total filas: 151</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>11:57</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,12 +3187,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:57</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3201,7 +3201,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,12 +3237,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3251,7 +3251,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3312,12 +3312,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3326,7 +3326,7 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3367,16 +3367,16 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,12 +3387,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3401,7 +3401,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,21 +3412,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,12 +3437,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3451,7 +3451,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,21 +3462,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,7 +3487,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3497,11 +3497,11 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,12 +3512,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3526,7 +3526,7 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,12 +3562,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3576,7 +3576,7 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,21 +3587,21 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,12 +3637,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3651,7 +3651,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,7 +3662,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3672,11 +3672,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,21 +3737,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3772,7 +3772,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D137" t="n">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3812,12 +3812,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3826,7 +3826,7 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3887,21 +3887,21 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,21 +3912,21 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3967,16 +3967,16 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3987,21 +3987,21 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>13:12</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,12 +4012,12 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:12</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4026,7 +4026,7 @@
         </is>
       </c>
       <c r="D147" t="n">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4037,21 +4037,21 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>13:16</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4062,12 +4062,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:16</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="D149" t="n">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4087,21 +4087,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4112,21 +4112,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:22</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4142,16 +4142,16 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4167,16 +4167,16 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4187,23 +4187,73 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>118</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>106</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
           <t>11:52:01</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
+      <c r="B156" t="inlineStr">
         <is>
           <t>13:47</t>
         </is>
       </c>
-      <c r="C154" t="inlineStr">
+      <c r="C156" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D154" t="n">
+      <c r="D156" t="n">
         <v>115</v>
       </c>
-      <c r="E154" t="inlineStr">
+      <c r="E156" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4238,7 +4288,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:52:01</t>
+          <t>Última actualización: 11:54:18</t>
         </is>
       </c>
     </row>
@@ -4955,7 +5005,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:52:01</t>
+          <t>Última actualización: 11:54:18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 151
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:54:18</t>
+          <t>Última actualización: 12:11:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 151</t>
+          <t>Total filas: 157</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1172,11 +1172,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1197,11 +1197,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>12:16</t>
+          <t>12:11</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3412,21 +3412,21 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>12:17</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3442,16 +3442,16 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:16</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3467,16 +3467,16 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,21 +3487,21 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3512,21 +3512,21 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:22</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3542,16 +3542,16 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,21 +3562,21 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:32</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,12 +3587,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>12:34</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3601,7 +3601,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,21 +3612,21 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:33</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3637,21 +3637,21 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:34</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3662,21 +3662,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3692,16 +3692,16 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,12 +3712,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3726,7 +3726,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,12 +3737,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3751,7 +3751,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,21 +3762,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,21 +3787,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3837,12 +3837,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3851,7 +3851,7 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,12 +3862,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3876,7 +3876,7 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>118</v>
+        <v>61</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3917,16 +3917,16 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,21 +3937,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3962,12 +3962,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -3976,7 +3976,7 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3987,12 +3987,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4001,7 +4001,7 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,21 +4012,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>13:12</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4042,16 +4042,16 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>13:13</t>
+          <t>13:04</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4067,16 +4067,16 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>13:16</t>
+          <t>13:12</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4092,16 +4092,16 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4112,21 +4112,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>13:22</t>
+          <t>13:16</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4137,21 +4137,21 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4162,21 +4162,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:22</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4192,16 +4192,16 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4217,16 +4217,16 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4237,23 +4237,173 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
+          <t>12:11:52</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>74</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>118</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>12:11:52</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>81</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>106</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>12:11:52</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>95</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
           <t>11:52:01</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr">
+      <c r="B161" t="inlineStr">
         <is>
           <t>13:47</t>
         </is>
       </c>
-      <c r="C156" t="inlineStr">
+      <c r="C161" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D156" t="n">
+      <c r="D161" t="n">
         <v>115</v>
       </c>
-      <c r="E156" t="inlineStr">
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>12:11:52</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>14:01</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>110</v>
+      </c>
+      <c r="E162" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4288,7 +4438,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:54:18</t>
+          <t>Última actualización: 12:11:52</t>
         </is>
       </c>
     </row>
@@ -4987,7 +5137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5005,14 +5155,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:54:18</t>
+          <t>Última actualización: 12:11:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -5565,6 +5715,31 @@
       <c r="E26" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>12:11:52</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>105</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 152
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:11:52</t>
+          <t>Última actualización: 12:33:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 157</t>
+          <t>Total filas: 162</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3747,11 +3747,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4262,7 +4262,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4272,11 +4272,11 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4287,7 +4287,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4297,11 +4297,11 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4387,23 +4387,148 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>81</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
           <t>12:11:52</t>
         </is>
       </c>
-      <c r="B162" t="inlineStr">
+      <c r="B163" t="inlineStr">
         <is>
           <t>14:01</t>
         </is>
       </c>
-      <c r="C162" t="inlineStr">
+      <c r="C163" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D162" t="n">
+      <c r="D163" t="n">
         <v>110</v>
       </c>
-      <c r="E162" t="inlineStr">
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>14:02</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>89</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>104</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>104</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>14:32</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>119</v>
+      </c>
+      <c r="E167" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4438,7 +4563,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:11:52</t>
+          <t>Última actualización: 12:33:21</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5155,14 +5280,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:11:52</t>
+          <t>Última actualización: 12:33:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -5738,6 +5863,31 @@
         <v>105</v>
       </c>
       <c r="E27" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>84</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 153
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:33:21</t>
+          <t>Última actualización: 12:45:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 162</t>
+          <t>Total filas: 170</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3662,7 +3662,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3672,11 +3672,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,7 +3687,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3697,11 +3697,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -4162,21 +4162,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>13:22</t>
+          <t>13:18</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4187,21 +4187,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4212,21 +4212,21 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:22</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4237,21 +4237,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4262,21 +4262,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4287,21 +4287,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,12 +4312,12 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="D159" t="n">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4342,16 +4342,16 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,21 +4362,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4387,21 +4387,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4412,21 +4412,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:47</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4442,16 +4442,16 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>14:02</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4462,21 +4462,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4487,21 +4487,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4517,18 +4517,218 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
+          <t>14:02</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>89</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>14:16</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>91</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>104</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>104</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>14:27</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>102</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>14:31</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>106</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
           <t>14:32</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr">
+      <c r="C173" t="inlineStr">
         <is>
           <t>14X44_ABASTO</t>
         </is>
       </c>
-      <c r="D167" t="n">
+      <c r="D173" t="n">
         <v>119</v>
       </c>
-      <c r="E167" t="inlineStr">
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>108</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>114</v>
+      </c>
+      <c r="E175" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4545,7 +4745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4563,14 +4763,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:33:21</t>
+          <t>Última actualización: 12:45:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 27</t>
         </is>
       </c>
     </row>
@@ -5246,6 +5446,31 @@
         <v>106</v>
       </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>108</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5280,7 +5505,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:33:21</t>
+          <t>Última actualización: 12:45:56</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 154
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E175"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:45:56</t>
+          <t>Última actualización: 12:52:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 170</t>
+          <t>Total filas: 174</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3747,11 +3747,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4187,21 +4187,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:19</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4212,12 +4212,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>13:22</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4226,7 +4226,7 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4237,21 +4237,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:22</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4262,12 +4262,12 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -4276,7 +4276,7 @@
         </is>
       </c>
       <c r="D157" t="n">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4287,7 +4287,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4297,11 +4297,11 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,21 +4312,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:25</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4337,7 +4337,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4347,11 +4347,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,21 +4362,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4387,21 +4387,21 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4412,12 +4412,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4426,7 +4426,7 @@
         </is>
       </c>
       <c r="D163" t="n">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4437,21 +4437,21 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:47</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4462,21 +4462,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4487,7 +4487,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -4497,11 +4497,11 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4512,21 +4512,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>14:02</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,21 +4537,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4562,21 +4562,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:09</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,12 +4587,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -4601,7 +4601,7 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4612,21 +4612,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4637,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4662,21 +4662,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4692,16 +4692,16 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4712,23 +4712,123 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
+          <t>12:33:21</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>14:32</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>119</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
           <t>12:45:56</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>108</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
         <is>
           <t>14:39</t>
         </is>
       </c>
-      <c r="C175" t="inlineStr">
+      <c r="C177" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D175" t="n">
+      <c r="D177" t="n">
         <v>114</v>
       </c>
-      <c r="E175" t="inlineStr">
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>12:52:52</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>115</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>12:52:52</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>119</v>
+      </c>
+      <c r="E179" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4745,7 +4845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4763,14 +4863,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:45:56</t>
+          <t>Última actualización: 12:52:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 27</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -5471,6 +5571,31 @@
         <v>108</v>
       </c>
       <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>12:52:52</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>115</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5505,7 +5630,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:45:56</t>
+          <t>Última actualización: 12:52:52</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 155
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:52:52</t>
+          <t>Última actualización: 13:14:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 174</t>
+          <t>Total filas: 181</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4562,21 +4562,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>14:09</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,21 +4587,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4612,21 +4612,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:09</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4637,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4662,21 +4662,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4687,21 +4687,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4712,21 +4712,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4742,16 +4742,16 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4762,21 +4762,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,21 +4787,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4812,23 +4812,198 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>80</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>114</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
           <t>12:52:52</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr">
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>115</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>12:52:52</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
         <is>
           <t>14:51</t>
         </is>
       </c>
-      <c r="C179" t="inlineStr">
+      <c r="C182" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D179" t="n">
+      <c r="D182" t="n">
         <v>119</v>
       </c>
-      <c r="E179" t="inlineStr">
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>100</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>108</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>15:12</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>118</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>119</v>
+      </c>
+      <c r="E186" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4845,7 +5020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4863,14 +5038,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:52:52</t>
+          <t>Última actualización: 13:14:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -5579,23 +5754,73 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>80</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>12:52:52</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B34" t="inlineStr">
         <is>
           <t>14:47</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D33" t="n">
+      <c r="D34" t="n">
         <v>115</v>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>100</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5612,7 +5837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5630,14 +5855,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:52:52</t>
+          <t>Última actualización: 13:14:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -6238,6 +6463,31 @@
         <v>84</v>
       </c>
       <c r="E28" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>79</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 156
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E186"/>
+  <dimension ref="A1:E196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:14:29</t>
+          <t>Última actualización: 13:41:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 181</t>
+          <t>Total filas: 191</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2272,11 +2272,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4412,21 +4412,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:43</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4437,12 +4437,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -4451,7 +4451,7 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4462,21 +4462,21 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>13:54</t>
+          <t>13:47</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4487,21 +4487,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>14:01</t>
+          <t>13:54</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,21 +4537,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>14:02</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4562,7 +4562,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4572,11 +4572,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4592,16 +4592,16 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>14:07</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4612,12 +4612,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>14:09</t>
+          <t>14:06</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -4626,7 +4626,7 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4637,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>14:07</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4662,21 +4662,21 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:09</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4687,21 +4687,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:14</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4717,16 +4717,16 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,21 +4737,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4767,16 +4767,16 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4792,16 +4792,16 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4812,21 +4812,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4842,16 +4842,16 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4862,21 +4862,21 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4887,21 +4887,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4917,16 +4917,16 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4937,21 +4937,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:39</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4962,21 +4962,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>15:12</t>
+          <t>14:47</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4987,23 +4987,273 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
         <v>119</v>
       </c>
       <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>14:51</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>70</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>72</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>100</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>80</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>15:02</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>108</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>15:12</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>118</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>17X38_ROMERO</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>119</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>93</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>111</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>112</v>
+      </c>
+      <c r="E196" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5020,7 +5270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5038,14 +5288,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:14:29</t>
+          <t>Última actualización: 13:41:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -5804,23 +6054,73 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>72</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>13:14:29</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B36" t="inlineStr">
         <is>
           <t>14:54</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D35" t="n">
+      <c r="D36" t="n">
         <v>100</v>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>112</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5837,7 +6137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5855,14 +6155,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:14:29</t>
+          <t>Última actualización: 13:41:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -6471,25 +6771,75 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:28</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>47</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>13:14:29</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>14:33</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D30" t="n">
         <v>79</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>100</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 157
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E196"/>
+  <dimension ref="A1:E203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:41:54</t>
+          <t>Última actualización: 13:56:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 191</t>
+          <t>Total filas: 198</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4547,11 +4547,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4787,21 +4787,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>14:18</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4812,12 +4812,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>14:28</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -4826,7 +4826,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4837,21 +4837,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>14:31</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4862,12 +4862,12 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>14:32</t>
+          <t>14:31</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -4876,7 +4876,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4887,21 +4887,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4912,12 +4912,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -4926,7 +4926,7 @@
         </is>
       </c>
       <c r="D183" t="n">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4937,21 +4937,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:34</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4962,21 +4962,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>14:39</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4992,16 +4992,16 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:47</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,21 +5012,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5037,21 +5037,21 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5062,21 +5062,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:51</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5092,16 +5092,16 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5117,16 +5117,16 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>15:02</t>
+          <t>14:54</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5137,21 +5137,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>15:12</t>
+          <t>15:01</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5167,16 +5167,16 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:02</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>17X38_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,12 +5187,12 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>15:14</t>
+          <t>15:12</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -5201,7 +5201,7 @@
         </is>
       </c>
       <c r="D194" t="n">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5212,21 +5212,21 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17X38_ROMERO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5242,18 +5242,193 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>93</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>15:18</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>82</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>111</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
           <t>15:33</t>
         </is>
       </c>
-      <c r="C196" t="inlineStr">
+      <c r="C199" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D196" t="n">
+      <c r="D199" t="n">
         <v>112</v>
       </c>
-      <c r="E196" t="inlineStr">
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>98</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>15:42</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>106</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>117</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>117</v>
+      </c>
+      <c r="E203" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5270,7 +5445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5288,14 +5463,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:41:54</t>
+          <t>Última actualización: 13:56:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -6054,21 +6229,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -6079,12 +6254,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -6093,7 +6268,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -6104,23 +6279,73 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>13:41:54</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B38" t="inlineStr">
         <is>
           <t>15:33</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="D38" t="n">
         <v>112</v>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>98</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6137,7 +6362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6155,14 +6380,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:41:54</t>
+          <t>Última actualización: 13:56:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -6521,7 +6746,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6531,11 +6756,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -6546,7 +6771,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:52:50</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -6556,11 +6781,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -6771,12 +6996,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>14:28</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -6785,7 +7010,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -6796,12 +7021,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -6810,7 +7035,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -6821,23 +7046,73 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>79</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>13:41:54</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>15:21</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="D32" t="n">
         <v>100</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:22</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>86</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 158
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E203"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:56:11</t>
+          <t>Última actualización: 14:12:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 198</t>
+          <t>Total filas: 204</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3662,7 +3662,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3672,11 +3672,11 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,7 +3687,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3697,11 +3697,11 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4287,7 +4287,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4297,11 +4297,11 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,7 +4312,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4322,11 +4322,11 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -5262,12 +5262,12 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>15:18</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -5276,7 +5276,7 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,21 +5287,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:18</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,21 +5312,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>15:33</t>
+          <t>15:29</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5337,21 +5337,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5362,21 +5362,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>15:42</t>
+          <t>15:33</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5392,16 +5392,16 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5412,23 +5412,173 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>84</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>15:41</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>89</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
           <t>13:56:11</t>
         </is>
       </c>
-      <c r="B203" t="inlineStr">
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>15:42</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>106</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
         <is>
           <t>15:53</t>
         </is>
       </c>
-      <c r="C203" t="inlineStr">
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>117</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D203" t="n">
+      <c r="D207" t="n">
         <v>117</v>
       </c>
-      <c r="E203" t="inlineStr">
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>104</v>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>113</v>
+      </c>
+      <c r="E209" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5463,7 +5613,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:56:11</t>
+          <t>Última actualización: 14:12:26</t>
         </is>
       </c>
     </row>
@@ -6362,7 +6512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6380,14 +6530,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:56:11</t>
+          <t>Última actualización: 14:12:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -6746,7 +6896,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08:52:50</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6756,11 +6906,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -6771,7 +6921,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -6781,11 +6931,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -7115,6 +7265,31 @@
       <c r="E33" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:02</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>110</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 159
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E209"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:12:26</t>
+          <t>Última actualización: 14:32:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 204</t>
+          <t>Total filas: 209</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3022,11 +3022,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3072,11 +3072,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3097,11 +3097,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3747,11 +3747,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -5262,21 +5262,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>15:17</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,12 +5287,12 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>15:18</t>
+          <t>15:17</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -5301,7 +5301,7 @@
         </is>
       </c>
       <c r="D198" t="n">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,21 +5312,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>15:29</t>
+          <t>15:18</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5337,21 +5337,21 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:29</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5367,16 +5367,16 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>15:33</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5387,12 +5387,12 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>15:33</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -5401,7 +5401,7 @@
         </is>
       </c>
       <c r="D202" t="n">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5412,21 +5412,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5442,16 +5442,16 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>15:41</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5462,12 +5462,12 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>15:42</t>
+          <t>15:41</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -5476,7 +5476,7 @@
         </is>
       </c>
       <c r="D205" t="n">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5492,16 +5492,16 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:42</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5522,7 +5522,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -5537,21 +5537,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5562,23 +5562,148 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>15:55</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>83</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
           <t>14:12:26</t>
         </is>
       </c>
-      <c r="B209" t="inlineStr">
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>104</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
         <is>
           <t>16:05</t>
         </is>
       </c>
-      <c r="C209" t="inlineStr">
+      <c r="C211" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D209" t="n">
+      <c r="D211" t="n">
         <v>113</v>
       </c>
-      <c r="E209" t="inlineStr">
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>102</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>105</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>109</v>
+      </c>
+      <c r="E214" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5613,7 +5738,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:12:26</t>
+          <t>Última actualización: 14:32:38</t>
         </is>
       </c>
     </row>
@@ -6512,7 +6637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6530,14 +6655,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:12:26</t>
+          <t>Última actualización: 14:32:38</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
     </row>
@@ -7271,25 +7396,75 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>89</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>14:12:26</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>16:02</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D35" t="n">
         <v>110</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>117</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 160
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:32:38</t>
+          <t>Última actualización: 14:45:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 209</t>
+          <t>Total filas: 213</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -5512,21 +5512,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:50</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5537,21 +5537,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:52</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5562,21 +5562,21 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,21 +5587,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5612,21 +5612,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5637,21 +5637,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5662,21 +5662,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5692,18 +5692,118 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>102</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>105</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
           <t>16:21</t>
         </is>
       </c>
-      <c r="C214" t="inlineStr">
+      <c r="C216" t="inlineStr">
         <is>
           <t>23_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D214" t="n">
+      <c r="D216" t="n">
         <v>109</v>
       </c>
-      <c r="E214" t="inlineStr">
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>14:45:56</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>108</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>14:45:56</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>115</v>
+      </c>
+      <c r="E218" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5738,7 +5838,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:32:38</t>
+          <t>Última actualización: 14:45:56</t>
         </is>
       </c>
     </row>
@@ -6637,7 +6737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6655,14 +6755,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:32:38</t>
+          <t>Última actualización: 14:45:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -7446,23 +7546,48 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>14:45:56</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:05</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>80</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>14:32:38</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>16:29</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D36" t="n">
+      <c r="D37" t="n">
         <v>117</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 161
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E218"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:45:56</t>
+          <t>Última actualización: 14:53:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 213</t>
+          <t>Total filas: 221</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5612,21 +5612,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5637,12 +5637,12 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -5651,7 +5651,7 @@
         </is>
       </c>
       <c r="D212" t="n">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5667,16 +5667,16 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5687,21 +5687,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>15:57</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5712,21 +5712,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5737,21 +5737,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,21 +5762,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5787,23 +5787,223 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>102</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>16:17</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>105</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>14:53:07</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>87</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>109</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
           <t>14:45:56</t>
         </is>
       </c>
-      <c r="B218" t="inlineStr">
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>16:33</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>108</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>14:53:07</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>83_ALUAR</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>101</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>14:45:56</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
         <is>
           <t>16:40</t>
         </is>
       </c>
-      <c r="C218" t="inlineStr">
+      <c r="C224" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D218" t="n">
+      <c r="D224" t="n">
         <v>115</v>
       </c>
-      <c r="E218" t="inlineStr">
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>14:53:07</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>108</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>14:53:07</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>16:46</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>113</v>
+      </c>
+      <c r="E226" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5838,7 +6038,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:45:56</t>
+          <t>Última actualización: 14:53:07</t>
         </is>
       </c>
     </row>
@@ -6737,7 +6937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6755,14 +6955,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:45:56</t>
+          <t>Última actualización: 14:53:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -7588,6 +7788,31 @@
         <v>117</v>
       </c>
       <c r="E37" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>14:53:07</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>97</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 162
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:53:07</t>
+          <t>Última actualización: 15:17:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 221</t>
+          <t>Total filas: 227</t>
         </is>
       </c>
     </row>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1172,11 +1172,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1197,11 +1197,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4337,7 +4337,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4347,11 +4347,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4372,11 +4372,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -5037,7 +5037,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5047,11 +5047,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5062,7 +5062,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5072,11 +5072,11 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5737,21 +5737,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5767,16 +5767,16 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5787,21 +5787,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5817,16 +5817,16 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5837,21 +5837,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5862,12 +5862,12 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -5876,7 +5876,7 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5887,21 +5887,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5912,21 +5912,21 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5942,16 +5942,16 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5967,16 +5967,16 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5987,23 +5987,173 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
+          <t>14:45:56</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>115</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
           <t>14:53:07</t>
         </is>
       </c>
-      <c r="B226" t="inlineStr">
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>16:41</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>108</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>14:53:07</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
         <is>
           <t>16:46</t>
         </is>
       </c>
-      <c r="C226" t="inlineStr">
+      <c r="C228" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D226" t="n">
+      <c r="D228" t="n">
         <v>113</v>
       </c>
-      <c r="E226" t="inlineStr">
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>96</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>101</v>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>110</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>113</v>
+      </c>
+      <c r="E232" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6015,6 +6165,948 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 15:17:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 35</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:17</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>60</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>58</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>57</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>69</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>110</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:45:36</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:46</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>101</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>44</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>105</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>80</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:52:50</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>66</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>109</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>85</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>96</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>104</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>71</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>89</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>77</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>118</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>106</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>108</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>80</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12:52:52</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>115</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:48</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>52</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>72</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>112</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>98</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>113</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6031,14 +7123,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:53:07</t>
+          <t>Última actualización: 15:17:33</t>
         </is>
       </c>
     </row>
@@ -6079,50 +7171,50 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>07:42</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:17</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -6134,195 +7226,195 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:54:04</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -6334,1487 +7426,595 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:46</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>08:52:50</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>10:31</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>13:11</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>13:12</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>15:22</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14:48</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>15:33</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 14:53:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 33</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>07:42</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>56</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05:57:13</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>106</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>08:35</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>109</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08:36</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>102</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>08:37</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>07:12:46</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>98</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
           <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>08:51</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>117</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>08:52</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>09:20</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>28</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>07:50:33</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>09:21</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>91</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>87</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:27:16</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>10:13</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>106</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>10:29</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>97</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>113</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>98</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10:31</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>106</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>10:05:51</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11:25</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>80</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>11:34:59</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>13:11</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>97</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>11:47:17</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>13:12</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>85</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>11:34:59</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>13:20</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>106</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>11:47:17</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>13:21</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>94</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>12:11:52</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>13:56</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>105</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:33:21</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:57</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>84</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>13:56:11</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>14:27</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>31</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>13:41:54</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>14:28</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>47</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>13:14:29</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>14:33</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>79</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>13:41:54</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>15:21</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>100</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>13:56:11</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>15:22</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>86</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>14:32:38</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>16:01</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>89</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>14:12:26</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>16:02</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>110</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>14:45:56</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>16:05</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>80</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>14:32:38</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>16:29</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>117</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>14:53:07</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>16:30</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>97</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 163
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E232"/>
+  <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:17:33</t>
+          <t>Última actualización: 15:46:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 227</t>
+          <t>Total filas: 236</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3022,11 +3022,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4547,11 +4547,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -5912,21 +5912,21 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5937,21 +5937,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5962,21 +5962,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5992,16 +5992,16 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6017,16 +6017,16 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6037,21 +6037,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6062,21 +6062,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6087,21 +6087,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:46</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6117,16 +6117,16 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6137,23 +6137,248 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>16:54</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>68</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
           <t>15:17:33</t>
         </is>
       </c>
-      <c r="B232" t="inlineStr">
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>16:58</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>101</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>17:07</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>110</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>17:09</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>83</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
         <is>
           <t>17:10</t>
         </is>
       </c>
-      <c r="C232" t="inlineStr">
+      <c r="C236" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D232" t="n">
+      <c r="D236" t="n">
         <v>113</v>
       </c>
-      <c r="E232" t="inlineStr">
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>95</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>108</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>111</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>113</v>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>116</v>
+      </c>
+      <c r="E241" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6165,6 +6390,998 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 15:46:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 37</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>06:16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>06:17</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:56</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:57</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>60</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>06:17:28</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>58</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:57:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:43</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>57</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>06:35:22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07:44</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>69</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:46:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>117</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:54:04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:44</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>110</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>08:45:36</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:46</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:53</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>101</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>44</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>07:12:46</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08:57</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>105</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07:38:39</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:58</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>80</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>08:52:50</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:58</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>66</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08:10:18</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>09:59</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>109</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>85</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:31</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:05:51</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>96</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10:37:52</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>104</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:11:33</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:22</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>71</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>89</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>77</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>11:34:59</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>118</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>11:47:17</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>13:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>106</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12:45:56</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:33</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>108</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:34</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>80</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12:52:52</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:47</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>115</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:48</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>52</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>72</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>13:14:29</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:54</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>13:41:54</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15:33</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>112</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>13:56:11</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>98</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>15:17:33</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>17:10</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>113</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>113</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>116</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6181,14 +7398,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 11/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:17:33</t>
+          <t>Última actualización: 15:46:07</t>
         </is>
       </c>
     </row>
@@ -6229,50 +7446,50 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:16</t>
+          <t>07:42</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:17</t>
+          <t>07:43</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -6284,195 +7501,195 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:56</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06:57</t>
+          <t>08:36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>08:37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>07:12:46</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>08:50</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:54:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07:43</t>
+          <t>08:51</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>06:35:22</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>08:52</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>09:20</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:54:04</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:44</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
@@ -6484,1535 +7701,618 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>08:46</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>10:13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>10:29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:12:46</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:57</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:52:50</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>08:52:50</t>
+          <t>08:45:36</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>09:58</t>
+          <t>10:31</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>11:25</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11:30</t>
+          <t>13:11</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>13:12</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>13:04</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>14:28</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13:33</t>
+          <t>14:33</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14:33</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14:34</t>
+          <t>15:22</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>14:47</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14:48</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>15:33</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15:34</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>LP1912</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="E40" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 11/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 15:17:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 34</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Linea</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Parada</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>07:42</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>56</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05:57:13</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>07:43</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>106</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06:46:50</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>08:35</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>109</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08:36</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>102</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>08:37</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>07:12:46</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:50</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>98</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>06:54:04</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>08:51</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>117</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>08:52</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>09:20</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>28</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>07:50:33</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>09:21</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>91</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>10:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>87</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>08:27:16</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>10:13</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>106</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>10:29</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>97</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>08:37:25</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>113</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>08:52:50</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>10:30</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>98</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>08:45:36</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10:31</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>106</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>10:05:51</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>11:25</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>80</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>11:34:59</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>13:11</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>97</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>11:47:17</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>13:12</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>85</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>11:34:59</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>13:20</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>106</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>11:47:17</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>13:21</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>94</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>12:11:52</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>13:56</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>105</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>12:33:21</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>13:57</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>84</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>13:56:11</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>14:27</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>31</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>13:41:54</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>14:28</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>47</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>13:14:29</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>14:33</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>79</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>13:41:54</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>15:21</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>100</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>13:56:11</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>15:22</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>86</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>14:32:38</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>16:01</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>89</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>14:12:26</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>16:02</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>110</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>14:45:56</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>16:05</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>80</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>L6203</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>14:32:38</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>16:29</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>117</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>14:53:07</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>16:30</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>97</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>L6173</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>15:17:33</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>17:05</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>108</v>
-      </c>
-      <c r="E39" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 164
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E241"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:46:07</t>
+          <t>Última actualización: 15:58:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 236</t>
+          <t>Total filas: 239</t>
         </is>
       </c>
     </row>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1172,11 +1172,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1197,11 +1197,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3022,11 +3022,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4562,7 +4562,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4572,11 +4572,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4597,11 +4597,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -5712,21 +5712,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>16:05</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5737,7 +5737,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5747,11 +5747,11 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,21 +5762,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>16:06</t>
+          <t>16:05</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5792,16 +5792,16 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:06</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5812,21 +5812,21 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5842,16 +5842,16 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5862,21 +5862,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5887,12 +5887,12 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -5901,7 +5901,7 @@
         </is>
       </c>
       <c r="D222" t="n">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5912,12 +5912,12 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -5926,7 +5926,7 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5937,21 +5937,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5962,7 +5962,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -5972,11 +5972,11 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5987,21 +5987,21 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6012,12 +6012,12 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -6026,7 +6026,7 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6037,21 +6037,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6062,12 +6062,12 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -6076,7 +6076,7 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6092,16 +6092,16 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6112,21 +6112,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:46</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6137,12 +6137,12 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -6151,7 +6151,7 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6162,21 +6162,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6192,16 +6192,16 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6212,21 +6212,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6237,21 +6237,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6262,21 +6262,21 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6292,16 +6292,16 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6317,16 +6317,16 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6337,21 +6337,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6367,18 +6367,93 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>111</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>113</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
           <t>17:42</t>
         </is>
       </c>
-      <c r="C241" t="inlineStr">
+      <c r="C243" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D241" t="n">
+      <c r="D243" t="n">
         <v>116</v>
       </c>
-      <c r="E241" t="inlineStr">
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>108</v>
+      </c>
+      <c r="E244" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6395,7 +6470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6413,14 +6488,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:46:07</t>
+          <t>Última actualización: 15:58:05</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -7371,6 +7446,31 @@
         <v>116</v>
       </c>
       <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>17:46</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>108</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7405,7 +7505,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:46:07</t>
+          <t>Última actualización: 15:58:05</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 165
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:58:05</t>
+          <t>Última actualización: 16:14:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 239</t>
+          <t>Total filas: 251</t>
         </is>
       </c>
     </row>
@@ -3587,7 +3587,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -4337,7 +4337,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4347,11 +4347,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4372,11 +4372,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D210" t="n">
@@ -5612,7 +5612,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5622,11 +5622,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5862,21 +5862,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5887,21 +5887,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5912,12 +5912,12 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>14:32:38</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -5926,7 +5926,7 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5937,12 +5937,12 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>14:32:38</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -5951,7 +5951,7 @@
         </is>
       </c>
       <c r="D224" t="n">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5962,21 +5962,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5987,12 +5987,12 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -6001,7 +6001,7 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6012,21 +6012,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6037,21 +6037,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6067,16 +6067,16 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6092,16 +6092,16 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6112,21 +6112,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6137,21 +6137,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6162,21 +6162,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:46</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6192,16 +6192,16 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6212,21 +6212,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6237,21 +6237,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6267,16 +6267,16 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6287,21 +6287,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6312,21 +6312,21 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6337,21 +6337,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6367,16 +6367,16 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,17 +6387,17 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D242" t="n">
@@ -6417,16 +6417,16 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6437,23 +6437,323 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>78</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>108</v>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
           <t>15:58:05</t>
         </is>
       </c>
-      <c r="B244" t="inlineStr">
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>98</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>17:37</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>111</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>84</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>113</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>116</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>91</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>15:58:05</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
         <is>
           <t>17:46</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
+      <c r="C252" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D244" t="n">
+      <c r="D252" t="n">
         <v>108</v>
       </c>
-      <c r="E244" t="inlineStr">
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>106</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>111</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>116</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>116</v>
+      </c>
+      <c r="E256" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6470,7 +6770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6488,14 +6788,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:58:05</t>
+          <t>Última actualización: 16:14:44</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -7379,12 +7679,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -7393,7 +7693,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -7404,17 +7704,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -7429,21 +7729,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -7454,23 +7754,98 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>17:39</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>113</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>15:46:07</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>116</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>91</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>15:58:05</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>17:46</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D46" t="n">
         <v>108</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7505,7 +7880,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:58:05</t>
+          <t>Última actualización: 16:14:44</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 166
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E256"/>
+  <dimension ref="A1:E266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:14:44</t>
+          <t>Última actualización: 16:28:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 251</t>
+          <t>Total filas: 261</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3747,11 +3747,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4547,11 +4547,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -5737,7 +5737,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5747,11 +5747,11 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,7 +5762,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -5772,11 +5772,11 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5987,12 +5987,12 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:28</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -6001,7 +6001,7 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6012,21 +6012,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6037,7 +6037,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6047,11 +6047,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6062,21 +6062,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>16:33</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>83_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6087,12 +6087,12 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>16:34</t>
+          <t>16:33</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -6101,7 +6101,7 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6112,21 +6112,21 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>14:45:56</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:34</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>83_ALUAR</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6137,12 +6137,12 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>14:45:56</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>16:41</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -6151,7 +6151,7 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6167,16 +6167,16 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>16:46</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6187,21 +6187,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:46</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6212,12 +6212,12 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>16:54</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -6226,7 +6226,7 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6237,21 +6237,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>16:54</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6262,21 +6262,21 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>16:58</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6287,21 +6287,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>17:03</t>
+          <t>16:58</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6312,21 +6312,21 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:03</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6337,21 +6337,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6362,21 +6362,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,21 +6387,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6412,21 +6412,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6437,21 +6437,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6467,16 +6467,16 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6487,12 +6487,12 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -6501,7 +6501,7 @@
         </is>
       </c>
       <c r="D246" t="n">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6512,12 +6512,12 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -6526,7 +6526,7 @@
         </is>
       </c>
       <c r="D247" t="n">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6537,21 +6537,21 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6562,21 +6562,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6592,16 +6592,16 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6617,16 +6617,16 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6637,21 +6637,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6662,21 +6662,21 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6692,16 +6692,16 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6712,21 +6712,21 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6737,23 +6737,273 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>17:49</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>81</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>17:53</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>85</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>17:58</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>90</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
           <t>16:14:44</t>
         </is>
       </c>
-      <c r="B256" t="inlineStr">
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>106</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>111</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>98</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
         <is>
           <t>18:10</t>
         </is>
       </c>
-      <c r="C256" t="inlineStr">
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>116</v>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>16:14:44</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D256" t="n">
+      <c r="D263" t="n">
         <v>116</v>
       </c>
-      <c r="E256" t="inlineStr">
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>109</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>114</v>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>117</v>
+      </c>
+      <c r="E266" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6770,7 +7020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6788,14 +7038,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:14:44</t>
+          <t>Última actualización: 16:28:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -7846,6 +8096,31 @@
         <v>108</v>
       </c>
       <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>114</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7880,7 +8155,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:14:44</t>
+          <t>Última actualización: 16:28:03</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 167
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E266"/>
+  <dimension ref="A1:E270"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:28:03</t>
+          <t>Última actualización: 16:37:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 261</t>
+          <t>Total filas: 265</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4562,7 +4562,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4572,11 +4572,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4597,11 +4597,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6762,21 +6762,21 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6787,21 +6787,21 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6812,12 +6812,12 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -6826,7 +6826,7 @@
         </is>
       </c>
       <c r="D259" t="n">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6837,21 +6837,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6862,21 +6862,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6892,16 +6892,16 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6912,21 +6912,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6937,21 +6937,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6962,21 +6962,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6992,18 +6992,118 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
+          <t>18:17</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>109</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>114</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
           <t>18:25</t>
         </is>
       </c>
-      <c r="C266" t="inlineStr">
+      <c r="C268" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D266" t="n">
+      <c r="D268" t="n">
         <v>117</v>
       </c>
-      <c r="E266" t="inlineStr">
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>16:37:06</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>113</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>16:37:06</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>119</v>
+      </c>
+      <c r="E270" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7038,7 +7138,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:28:03</t>
+          <t>Última actualización: 16:37:06</t>
         </is>
       </c>
     </row>
@@ -8137,7 +8237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8155,14 +8255,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:28:03</t>
+          <t>Última actualización: 16:37:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -9063,6 +9163,31 @@
         <v>80</v>
       </c>
       <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>16:37:06</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>119</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 168
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E270"/>
+  <dimension ref="A1:E272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:37:06</t>
+          <t>Última actualización: 16:44:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 265</t>
+          <t>Total filas: 267</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3022,11 +3022,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -6387,12 +6387,12 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:44:12</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:08</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -6401,7 +6401,7 @@
         </is>
       </c>
       <c r="D242" t="n">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6437,21 +6437,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6462,21 +6462,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6487,21 +6487,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6512,12 +6512,12 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -6526,7 +6526,7 @@
         </is>
       </c>
       <c r="D247" t="n">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6537,21 +6537,21 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6562,21 +6562,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6587,12 +6587,12 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -6601,7 +6601,7 @@
         </is>
       </c>
       <c r="D250" t="n">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,21 +6612,21 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6637,12 +6637,12 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -6651,7 +6651,7 @@
         </is>
       </c>
       <c r="D252" t="n">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6667,16 +6667,16 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6687,12 +6687,12 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -6701,7 +6701,7 @@
         </is>
       </c>
       <c r="D254" t="n">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6712,12 +6712,12 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -6726,7 +6726,7 @@
         </is>
       </c>
       <c r="D255" t="n">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6737,21 +6737,21 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6762,12 +6762,12 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:44:12</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -6776,7 +6776,7 @@
         </is>
       </c>
       <c r="D257" t="n">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6787,21 +6787,21 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6812,21 +6812,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6837,21 +6837,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6862,12 +6862,12 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -6876,7 +6876,7 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,21 +6887,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6912,21 +6912,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6942,16 +6942,16 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6962,21 +6962,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6987,21 +6987,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7012,21 +7012,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7042,16 +7042,16 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7062,21 +7062,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7087,23 +7087,73 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>117</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
           <t>16:37:06</t>
         </is>
       </c>
-      <c r="B270" t="inlineStr">
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>113</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>16:37:06</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
         <is>
           <t>18:36</t>
         </is>
       </c>
-      <c r="C270" t="inlineStr">
+      <c r="C272" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D270" t="n">
+      <c r="D272" t="n">
         <v>119</v>
       </c>
-      <c r="E270" t="inlineStr">
+      <c r="E272" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7138,7 +7188,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:37:06</t>
+          <t>Última actualización: 16:44:12</t>
         </is>
       </c>
     </row>
@@ -8255,7 +8305,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:37:06</t>
+          <t>Última actualización: 16:44:12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 169
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E272"/>
+  <dimension ref="A1:E277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:44:12</t>
+          <t>Última actualización: 16:52:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 267</t>
+          <t>Total filas: 272</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3022,11 +3022,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,7 +5587,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5597,11 +5597,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -6337,12 +6337,12 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -6351,7 +6351,7 @@
         </is>
       </c>
       <c r="D240" t="n">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6362,7 +6362,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6372,11 +6372,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>110</v>
+        <v>39</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,21 +6387,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>16:44:12</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>17:08</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6412,21 +6412,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:44:12</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:08</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6462,12 +6462,12 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -6476,7 +6476,7 @@
         </is>
       </c>
       <c r="D245" t="n">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6487,21 +6487,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6512,21 +6512,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6537,12 +6537,12 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -6551,7 +6551,7 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6562,21 +6562,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:32</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6587,21 +6587,21 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,12 +6612,12 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -6626,7 +6626,7 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6637,21 +6637,21 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D252" t="n">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6662,12 +6662,12 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -6676,7 +6676,7 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6692,16 +6692,16 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6712,12 +6712,12 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -6726,7 +6726,7 @@
         </is>
       </c>
       <c r="D255" t="n">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6737,12 +6737,12 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>17:46</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -6751,7 +6751,7 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6762,12 +6762,12 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:44:12</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>17:48</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -6776,7 +6776,7 @@
         </is>
       </c>
       <c r="D257" t="n">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6787,21 +6787,21 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:46</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6812,12 +6812,12 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:44:12</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -6826,7 +6826,7 @@
         </is>
       </c>
       <c r="D259" t="n">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6837,21 +6837,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6862,21 +6862,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,21 +6887,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6912,12 +6912,12 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -6926,7 +6926,7 @@
         </is>
       </c>
       <c r="D263" t="n">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6937,21 +6937,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6962,21 +6962,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6992,16 +6992,16 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7012,21 +7012,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7037,21 +7037,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7062,21 +7062,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7092,16 +7092,16 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7112,21 +7112,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7137,23 +7137,148 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>18:22</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>114</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>16:28:03</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>117</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>16:52:42</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>18:29</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>97</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
           <t>16:37:06</t>
         </is>
       </c>
-      <c r="B272" t="inlineStr">
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>113</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>16:37:06</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
         <is>
           <t>18:36</t>
         </is>
       </c>
-      <c r="C272" t="inlineStr">
+      <c r="C276" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D272" t="n">
+      <c r="D276" t="n">
         <v>119</v>
       </c>
-      <c r="E272" t="inlineStr">
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>16:52:42</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>113</v>
+      </c>
+      <c r="E277" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7170,7 +7295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7188,14 +7313,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:44:12</t>
+          <t>Última actualización: 16:52:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -8254,23 +8379,48 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>16:52:42</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>89</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>16:28:03</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>18:22</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="D48" t="n">
         <v>114</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8287,7 +8437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8305,14 +8455,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:44:12</t>
+          <t>Última actualización: 16:52:42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -9221,23 +9371,48 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>16:52:42</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>18:35</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>103</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>16:37:06</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>18:36</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D42" t="n">
         <v>119</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 170
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E277"/>
+  <dimension ref="A1:E284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:42</t>
+          <t>Última actualización: 17:13:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 272</t>
+          <t>Total filas: 279</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3072,11 +3072,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3097,11 +3097,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -6362,7 +6362,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6372,11 +6372,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,7 +6387,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6397,11 +6397,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>110</v>
+        <v>39</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6887,21 +6887,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6912,12 +6912,12 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -6926,7 +6926,7 @@
         </is>
       </c>
       <c r="D263" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6942,16 +6942,16 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6962,21 +6962,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6992,16 +6992,16 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7012,12 +7012,12 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -7026,7 +7026,7 @@
         </is>
       </c>
       <c r="D267" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7037,21 +7037,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7087,21 +7087,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7112,21 +7112,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7137,12 +7137,12 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -7151,7 +7151,7 @@
         </is>
       </c>
       <c r="D272" t="n">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7167,16 +7167,16 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7187,21 +7187,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7212,12 +7212,12 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -7226,7 +7226,7 @@
         </is>
       </c>
       <c r="D275" t="n">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7242,16 +7242,16 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7262,23 +7262,198 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
+          <t>16:37:06</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>119</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>18:36</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>83</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>18:41</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>88</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
           <t>16:52:42</t>
         </is>
       </c>
-      <c r="B277" t="inlineStr">
+      <c r="B280" t="inlineStr">
         <is>
           <t>18:45</t>
         </is>
       </c>
-      <c r="C277" t="inlineStr">
+      <c r="C280" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D277" t="n">
+      <c r="D280" t="n">
         <v>113</v>
       </c>
-      <c r="E277" t="inlineStr">
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>99</v>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>18:57</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>104</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>106</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>110</v>
+      </c>
+      <c r="E284" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7295,7 +7470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7313,14 +7488,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:42</t>
+          <t>Última actualización: 17:13:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -8421,6 +8596,31 @@
         <v>114</v>
       </c>
       <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>110</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8455,7 +8655,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:42</t>
+          <t>Última actualización: 17:13:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 171
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E284"/>
+  <dimension ref="A1:E290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:13:39</t>
+          <t>Última actualización: 17:36:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 279</t>
+          <t>Total filas: 285</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,7 +3587,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D209" t="n">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -6037,7 +6037,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -6047,11 +6047,11 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6062,7 +6062,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -6072,11 +6072,11 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -7312,21 +7312,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7337,21 +7337,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7362,21 +7362,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7392,16 +7392,16 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7417,16 +7417,16 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7442,18 +7442,168 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>106</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>84</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
           <t>19:03</t>
         </is>
       </c>
-      <c r="C284" t="inlineStr">
+      <c r="C286" t="inlineStr">
         <is>
           <t>215_EL PELIGRO</t>
         </is>
       </c>
-      <c r="D284" t="n">
+      <c r="D286" t="n">
         <v>110</v>
       </c>
-      <c r="E284" t="inlineStr">
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>88</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>101</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>101</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>112</v>
+      </c>
+      <c r="E290" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7470,7 +7620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7488,14 +7638,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:13:39</t>
+          <t>Última actualización: 17:36:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -8621,6 +8771,56 @@
         <v>110</v>
       </c>
       <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>88</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>112</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8637,7 +8837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8655,14 +8855,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:13:39</t>
+          <t>Última actualización: 17:36:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -9615,6 +9815,31 @@
       <c r="E42" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>108</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 172
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E290"/>
+  <dimension ref="A1:E296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:36:10</t>
+          <t>Última actualización: 17:48:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 285</t>
+          <t>Total filas: 291</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2272,11 +2272,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3587,7 +3587,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4337,7 +4337,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4347,11 +4347,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4372,11 +4372,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4562,7 +4562,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4572,11 +4572,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4597,11 +4597,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6837,21 +6837,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>17:49</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6862,21 +6862,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,12 +6887,12 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:49</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -6901,7 +6901,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6917,16 +6917,16 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6937,21 +6937,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6962,21 +6962,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6987,12 +6987,12 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -7001,7 +7001,7 @@
         </is>
       </c>
       <c r="D266" t="n">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7012,21 +7012,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7037,21 +7037,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7067,16 +7067,16 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7087,21 +7087,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7112,21 +7112,21 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7137,21 +7137,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7167,16 +7167,16 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7187,21 +7187,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7212,21 +7212,21 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7237,21 +7237,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7262,21 +7262,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7287,21 +7287,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7312,12 +7312,12 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>18:37</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -7326,7 +7326,7 @@
         </is>
       </c>
       <c r="D279" t="n">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7337,21 +7337,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7362,21 +7362,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7387,21 +7387,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7417,16 +7417,16 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7437,21 +7437,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7462,21 +7462,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7492,16 +7492,16 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7512,21 +7512,21 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7542,16 +7542,16 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7562,21 +7562,21 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7592,18 +7592,168 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>88</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>19:12</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>84</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>101</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>101</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
           <t>19:28</t>
         </is>
       </c>
-      <c r="C290" t="inlineStr">
+      <c r="C294" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D290" t="n">
+      <c r="D294" t="n">
         <v>112</v>
       </c>
-      <c r="E290" t="inlineStr">
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>107</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>111</v>
+      </c>
+      <c r="E296" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7620,7 +7770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7638,14 +7788,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:36:10</t>
+          <t>Última actualización: 17:48:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -8704,21 +8854,21 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -8729,21 +8879,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>17:48</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -8754,21 +8904,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -8779,21 +8929,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -8804,23 +8954,73 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>17:13:39</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>110</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>17:36:10</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>88</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>19:28</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D53" t="n">
         <v>112</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8855,7 +9055,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:36:10</t>
+          <t>Última actualización: 17:48:33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 173
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E296"/>
+  <dimension ref="A1:E304"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:48:33</t>
+          <t>Última actualización: 17:56:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 291</t>
+          <t>Total filas: 299</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1172,11 +1172,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1197,11 +1197,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3747,11 +3747,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,7 +5587,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5597,11 +5597,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -6812,7 +6812,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>16:44:12</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -6822,11 +6822,11 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6837,7 +6837,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>16:44:12</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -6847,11 +6847,11 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6872,7 +6872,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7012,21 +7012,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>17:58</t>
+          <t>17:56</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7037,21 +7037,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:57</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7062,21 +7062,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7087,21 +7087,21 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7117,16 +7117,16 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7137,21 +7137,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:06</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7162,21 +7162,21 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>18:17</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7187,21 +7187,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7217,16 +7217,16 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>18:17</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7237,21 +7237,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7262,21 +7262,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>18:29</t>
+          <t>18:22</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7287,21 +7287,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7312,21 +7312,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:29</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7342,16 +7342,16 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7362,12 +7362,12 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -7376,7 +7376,7 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7387,21 +7387,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>18:37</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7417,16 +7417,16 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7437,21 +7437,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7467,16 +7467,16 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7487,21 +7487,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7517,16 +7517,16 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7537,21 +7537,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7567,16 +7567,16 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7592,16 +7592,16 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7612,21 +7612,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7642,16 +7642,16 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7662,21 +7662,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7687,21 +7687,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7712,21 +7712,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7737,23 +7737,223 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>101</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>101</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>85</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>112</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
           <t>17:48:33</t>
         </is>
       </c>
-      <c r="B296" t="inlineStr">
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>107</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>100</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
         <is>
           <t>19:39</t>
         </is>
       </c>
-      <c r="C296" t="inlineStr">
+      <c r="C302" t="inlineStr">
         <is>
           <t>15X38_ABASTO</t>
         </is>
       </c>
-      <c r="D296" t="n">
+      <c r="D302" t="n">
         <v>111</v>
       </c>
-      <c r="E296" t="inlineStr">
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>116</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>117</v>
+      </c>
+      <c r="E304" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7788,7 +7988,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:48:33</t>
+          <t>Última actualización: 17:56:03</t>
         </is>
       </c>
     </row>
@@ -9055,7 +9255,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:48:33</t>
+          <t>Última actualización: 17:56:03</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 174
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E304"/>
+  <dimension ref="A1:E307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:56:03</t>
+          <t>Última actualización: 18:12:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 299</t>
+          <t>Total filas: 302</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>06:46:50</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1172,11 +1172,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>06:46:50</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1197,11 +1197,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3072,11 +3072,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3097,11 +3097,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -6362,7 +6362,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6372,11 +6372,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>110</v>
+        <v>39</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,7 +6387,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6397,11 +6397,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6822,7 +6822,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D259" t="n">
@@ -6872,7 +6872,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7687,21 +7687,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7712,21 +7712,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7737,21 +7737,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7762,21 +7762,21 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7787,21 +7787,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7817,16 +7817,16 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7837,21 +7837,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7862,21 +7862,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7887,21 +7887,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7912,21 +7912,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7942,18 +7942,93 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>100</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>111</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>116</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
           <t>19:53</t>
         </is>
       </c>
-      <c r="C304" t="inlineStr">
+      <c r="C307" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D304" t="n">
+      <c r="D307" t="n">
         <v>117</v>
       </c>
-      <c r="E304" t="inlineStr">
+      <c r="E307" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7988,7 +8063,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:56:03</t>
+          <t>Última actualización: 18:12:30</t>
         </is>
       </c>
     </row>
@@ -9237,7 +9312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9255,14 +9330,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:56:03</t>
+          <t>Última actualización: 18:12:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -10240,6 +10315,31 @@
       <c r="E43" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>18:12:30</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19:58</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>106</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 175
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E307"/>
+  <dimension ref="A1:E311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:12:30</t>
+          <t>Última actualización: 18:31:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 302</t>
+          <t>Total filas: 306</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05:57:13</t>
+          <t>06:17:28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -922,11 +922,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>06:17:28</t>
+          <t>05:57:13</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -947,11 +947,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3587,7 +3587,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4287,7 +4287,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4297,11 +4297,11 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,7 +4312,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4322,11 +4322,11 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4547,11 +4547,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -5737,7 +5737,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5747,11 +5747,11 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,7 +5762,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -5772,11 +5772,11 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -6437,7 +6437,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6447,11 +6447,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6462,7 +6462,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -6472,11 +6472,11 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D273" t="n">
@@ -7197,7 +7197,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D274" t="n">
@@ -7387,21 +7387,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7437,21 +7437,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>18:37</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7462,21 +7462,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>18:41</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7487,21 +7487,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>18:45</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7517,16 +7517,16 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:41</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7537,21 +7537,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7567,16 +7567,16 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7587,21 +7587,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7617,16 +7617,16 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7642,16 +7642,16 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7662,21 +7662,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7687,21 +7687,21 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7712,12 +7712,12 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -7726,7 +7726,7 @@
         </is>
       </c>
       <c r="D295" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7737,21 +7737,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7762,12 +7762,12 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -7776,7 +7776,7 @@
         </is>
       </c>
       <c r="D297" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7787,21 +7787,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7812,21 +7812,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7837,21 +7837,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7862,21 +7862,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7887,21 +7887,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7912,21 +7912,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7937,21 +7937,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7967,16 +7967,16 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7992,16 +7992,16 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8012,23 +8012,123 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>111</v>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
           <t>17:56:03</t>
         </is>
       </c>
-      <c r="B307" t="inlineStr">
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>116</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
         <is>
           <t>19:53</t>
         </is>
       </c>
-      <c r="C307" t="inlineStr">
+      <c r="C309" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D307" t="n">
+      <c r="D309" t="n">
         <v>117</v>
       </c>
-      <c r="E307" t="inlineStr">
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18:31:25</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>101</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>18:31:25</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>111</v>
+      </c>
+      <c r="E311" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8045,7 +8145,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8063,14 +8163,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:12:30</t>
+          <t>Última actualización: 18:31:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -9296,6 +9396,31 @@
         <v>112</v>
       </c>
       <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>18:31:25</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>101</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9330,7 +9455,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:12:30</t>
+          <t>Última actualización: 18:31:25</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 176
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E311"/>
+  <dimension ref="A1:E327"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:31:25</t>
+          <t>Última actualización: 18:44:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 306</t>
+          <t>Total filas: 322</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3747,11 +3747,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -5737,7 +5737,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5747,11 +5747,11 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,7 +5762,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -5772,11 +5772,11 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -6762,7 +6762,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6772,11 +6772,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6787,7 +6787,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6797,11 +6797,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -7562,12 +7562,12 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -7576,7 +7576,7 @@
         </is>
       </c>
       <c r="D289" t="n">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7592,16 +7592,16 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>18:57</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7612,21 +7612,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7637,21 +7637,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7667,16 +7667,16 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7692,16 +7692,16 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D294" t="n">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7712,21 +7712,21 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D295" t="n">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7737,21 +7737,21 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7762,12 +7762,12 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -7776,7 +7776,7 @@
         </is>
       </c>
       <c r="D297" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7787,21 +7787,21 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7812,12 +7812,12 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -7826,7 +7826,7 @@
         </is>
       </c>
       <c r="D299" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7837,21 +7837,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7862,21 +7862,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7887,21 +7887,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7912,21 +7912,21 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7942,16 +7942,16 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7962,21 +7962,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7992,16 +7992,16 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8012,21 +8012,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8037,21 +8037,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:23</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8062,21 +8062,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8087,21 +8087,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8112,23 +8112,423 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>112</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>107</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>100</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>19:38</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>54</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>17:48:33</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>15X38_ABASTO</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>111</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>67</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>116</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>19:52</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>68</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>17:56:03</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>117</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>69</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>20:06</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>82</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>20:09</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>85</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
           <t>18:31:25</t>
         </is>
       </c>
-      <c r="B311" t="inlineStr">
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>101</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>88</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>97</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18:31:25</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
         <is>
           <t>20:22</t>
         </is>
       </c>
-      <c r="C311" t="inlineStr">
+      <c r="C326" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D311" t="n">
+      <c r="D326" t="n">
         <v>111</v>
       </c>
-      <c r="E311" t="inlineStr">
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>106</v>
+      </c>
+      <c r="E327" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8145,7 +8545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8163,14 +8563,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:31:25</t>
+          <t>Última actualización: 18:44:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 49</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -9379,12 +9779,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -9393,7 +9793,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -9404,23 +9804,73 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>19:28</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>112</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>20:06</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>82</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>18:31:25</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B56" t="inlineStr">
         <is>
           <t>20:12</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D54" t="n">
+      <c r="D56" t="n">
         <v>101</v>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9437,7 +9887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9455,14 +9905,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:31:25</t>
+          <t>Última actualización: 18:44:57</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -10421,12 +10871,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>19:24</t>
+          <t>19:23</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -10435,7 +10885,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -10446,23 +10896,73 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>17:36:10</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19:24</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>108</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>19:57</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>73</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>18:12:30</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>19:58</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="D46" t="n">
         <v>106</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 177
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E327"/>
+  <dimension ref="A1:E333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:44:57</t>
+          <t>Última actualización: 18:52:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 322</t>
+          <t>Total filas: 328</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>07:50:33</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1947,11 +1947,11 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:50:33</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4547,11 +4547,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4562,7 +4562,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4572,11 +4572,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4597,11 +4597,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D210" t="n">
@@ -5612,7 +5612,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5622,11 +5622,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -7862,7 +7862,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -7872,11 +7872,11 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7887,7 +7887,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7897,11 +7897,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7912,7 +7912,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -7922,11 +7922,11 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -8137,21 +8137,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8162,12 +8162,12 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -8176,7 +8176,7 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8187,21 +8187,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>19:38</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8212,12 +8212,12 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:38</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -8226,7 +8226,7 @@
         </is>
       </c>
       <c r="D315" t="n">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8237,21 +8237,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8262,12 +8262,12 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -8276,7 +8276,7 @@
         </is>
       </c>
       <c r="D317" t="n">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8287,7 +8287,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -8297,11 +8297,11 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8312,12 +8312,12 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -8326,7 +8326,7 @@
         </is>
       </c>
       <c r="D319" t="n">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8367,16 +8367,16 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>20:06</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8392,16 +8392,16 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:06</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8412,12 +8412,12 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -8426,7 +8426,7 @@
         </is>
       </c>
       <c r="D323" t="n">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8437,21 +8437,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8467,16 +8467,16 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8487,21 +8487,21 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8512,23 +8512,173 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
+          <t>18:31:25</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>101</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>18:52:02</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>20:13</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>81</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
           <t>18:44:57</t>
         </is>
       </c>
-      <c r="B327" t="inlineStr">
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>97</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18:31:25</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>111</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18:44:57</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
         <is>
           <t>20:30</t>
         </is>
       </c>
-      <c r="C327" t="inlineStr">
+      <c r="C331" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D327" t="n">
+      <c r="D331" t="n">
         <v>106</v>
       </c>
-      <c r="E327" t="inlineStr">
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18:52:02</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>99</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>18:52:02</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>116</v>
+      </c>
+      <c r="E333" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8545,7 +8695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8563,14 +8713,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:44:57</t>
+          <t>Última actualización: 18:52:02</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 53</t>
         </is>
       </c>
     </row>
@@ -9854,23 +10004,73 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>18:52:02</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>20:07</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>75</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>18:31:25</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>20:12</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D56" t="n">
+      <c r="D57" t="n">
         <v>101</v>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>18:52:02</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>116</v>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9905,7 +10105,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:44:57</t>
+          <t>Última actualización: 18:52:02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 178
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E333"/>
+  <dimension ref="A1:E338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:02</t>
+          <t>Última actualización: 19:11:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 328</t>
+          <t>Total filas: 333</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>08:37:25</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2272,11 +2272,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>08:37:25</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,7 +2837,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2847,11 +2847,11 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3072,11 +3072,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3097,11 +3097,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3587,7 +3587,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -4337,7 +4337,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4347,11 +4347,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4372,11 +4372,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4562,7 +4562,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>12:33:21</t>
+          <t>13:14:29</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4572,11 +4572,11 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4587,7 +4587,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>13:14:29</t>
+          <t>12:33:21</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4597,11 +4597,11 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -6437,7 +6437,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6447,11 +6447,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6462,7 +6462,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -6472,11 +6472,11 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -7762,7 +7762,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7772,11 +7772,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7787,7 +7787,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -7797,11 +7797,11 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7837,21 +7837,21 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>19:15</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7867,16 +7867,16 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7887,7 +7887,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7897,11 +7897,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7912,7 +7912,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -7922,11 +7922,11 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7937,12 +7937,12 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -7951,7 +7951,7 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7972,7 +7972,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7987,21 +7987,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8012,12 +8012,12 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -8026,7 +8026,7 @@
         </is>
       </c>
       <c r="D307" t="n">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8037,21 +8037,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>19:23</t>
+          <t>19:22</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8067,16 +8067,16 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>19:27</t>
+          <t>19:23</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8112,12 +8112,12 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>17:36:10</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:27</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -8126,7 +8126,7 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8137,21 +8137,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>17:36:10</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8162,21 +8162,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8187,12 +8187,12 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -8201,7 +8201,7 @@
         </is>
       </c>
       <c r="D314" t="n">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8212,21 +8212,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>19:38</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8237,12 +8237,12 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:38</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -8251,7 +8251,7 @@
         </is>
       </c>
       <c r="D316" t="n">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8262,21 +8262,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8287,12 +8287,12 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -8301,7 +8301,7 @@
         </is>
       </c>
       <c r="D318" t="n">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8312,7 +8312,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8322,11 +8322,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,12 +8337,12 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -8351,7 +8351,7 @@
         </is>
       </c>
       <c r="D320" t="n">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8362,7 +8362,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -8372,11 +8372,11 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8392,16 +8392,16 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>20:06</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8412,12 +8412,12 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>20:06</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -8426,7 +8426,7 @@
         </is>
       </c>
       <c r="D323" t="n">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8442,16 +8442,16 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>20:08</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8462,12 +8462,12 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -8476,7 +8476,7 @@
         </is>
       </c>
       <c r="D325" t="n">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8492,16 +8492,16 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8512,7 +8512,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8522,11 +8522,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,21 +8537,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8562,21 +8562,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8587,12 +8587,12 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -8601,7 +8601,7 @@
         </is>
       </c>
       <c r="D330" t="n">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8612,21 +8612,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,12 +8637,12 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -8651,7 +8651,7 @@
         </is>
       </c>
       <c r="D332" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8667,18 +8667,143 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>99</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>92</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>96</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>18:52:02</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
           <t>20:48</t>
         </is>
       </c>
-      <c r="C333" t="inlineStr">
+      <c r="C336" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D333" t="n">
+      <c r="D336" t="n">
         <v>116</v>
       </c>
-      <c r="E333" t="inlineStr">
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>105</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>21:06</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>115</v>
+      </c>
+      <c r="E338" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8695,7 +8820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8713,14 +8838,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:02</t>
+          <t>Última actualización: 19:11:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 53</t>
+          <t>Total filas: 54</t>
         </is>
       </c>
     </row>
@@ -10054,23 +10179,48 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>96</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
           <t>18:52:02</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B59" t="inlineStr">
         <is>
           <t>20:48</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D58" t="n">
+      <c r="D59" t="n">
         <v>116</v>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10087,7 +10237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10105,14 +10255,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:52:02</t>
+          <t>Última actualización: 19:11:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -11163,6 +11313,31 @@
         <v>106</v>
       </c>
       <c r="E46" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>20:51</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>100</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 179
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E338"/>
+  <dimension ref="A1:E345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:11:45</t>
+          <t>Última actualización: 19:35:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 333</t>
+          <t>Total filas: 340</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>08:27:16</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1747,11 +1747,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:27:16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5737,7 +5737,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5747,11 +5747,11 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,7 +5762,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -5772,11 +5772,11 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -6762,7 +6762,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6772,11 +6772,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6787,7 +6787,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6797,11 +6797,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6822,7 +6822,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D259" t="n">
@@ -6872,7 +6872,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
@@ -7887,7 +7887,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7897,11 +7897,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7937,7 +7937,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -7947,11 +7947,11 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -8412,21 +8412,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>20:06</t>
+          <t>20:04</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8437,12 +8437,12 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>20:06</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -8451,7 +8451,7 @@
         </is>
       </c>
       <c r="D324" t="n">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8467,16 +8467,16 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>20:08</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8487,12 +8487,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -8501,7 +8501,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8517,16 +8517,16 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,7 +8537,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8547,11 +8547,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8562,21 +8562,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8587,21 +8587,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8612,12 +8612,12 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -8626,7 +8626,7 @@
         </is>
       </c>
       <c r="D331" t="n">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,21 +8637,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8662,12 +8662,12 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -8676,7 +8676,7 @@
         </is>
       </c>
       <c r="D333" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8687,21 +8687,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8712,21 +8712,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:33</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8737,21 +8737,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:42</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8767,16 +8767,16 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8792,18 +8792,193 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>96</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>18:52:02</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>20:48</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>116</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>105</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>19:35:56</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>82</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
           <t>21:06</t>
         </is>
       </c>
-      <c r="C338" t="inlineStr">
+      <c r="C342" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D338" t="n">
+      <c r="D342" t="n">
         <v>115</v>
       </c>
-      <c r="E338" t="inlineStr">
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>19:35:56</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>21:09</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>94</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>19:35:56</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>113</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>19:35:56</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>21:33</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>118</v>
+      </c>
+      <c r="E345" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8838,7 +9013,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:11:45</t>
+          <t>Última actualización: 19:35:56</t>
         </is>
       </c>
     </row>
@@ -10255,7 +10430,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:11:45</t>
+          <t>Última actualización: 19:35:56</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 180
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E345"/>
+  <dimension ref="A1:E355"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:35:56</t>
+          <t>Última actualización: 19:48:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 340</t>
+          <t>Total filas: 350</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>08:10:18</t>
+          <t>07:38:39</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1797,11 +1797,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>07:38:39</t>
+          <t>08:10:18</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:54:18</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,7 +3137,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>11:54:18</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3147,11 +3147,11 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,7 +3162,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3172,11 +3172,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3712,7 +3712,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3747,11 +3747,11 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4547,11 +4547,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -6762,7 +6762,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>16:52:42</t>
+          <t>15:58:05</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -6772,11 +6772,11 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6787,7 +6787,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>15:58:05</t>
+          <t>16:52:42</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -6797,11 +6797,11 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8287,21 +8287,21 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8312,12 +8312,12 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -8326,7 +8326,7 @@
         </is>
       </c>
       <c r="D319" t="n">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8362,12 +8362,12 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -8376,7 +8376,7 @@
         </is>
       </c>
       <c r="D321" t="n">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8387,7 +8387,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -8397,11 +8397,11 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8412,21 +8412,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>20:04</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8437,21 +8437,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>20:06</t>
+          <t>20:04</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8462,12 +8462,12 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>20:06</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -8476,7 +8476,7 @@
         </is>
       </c>
       <c r="D325" t="n">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8487,12 +8487,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:08</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -8501,7 +8501,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8512,21 +8512,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,21 +8537,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8562,21 +8562,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8587,12 +8587,12 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -8601,7 +8601,7 @@
         </is>
       </c>
       <c r="D330" t="n">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8612,21 +8612,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,21 +8637,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8667,16 +8667,16 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8687,21 +8687,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8712,21 +8712,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>20:33</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8737,21 +8737,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>20:42</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8762,21 +8762,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:33</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,21 +8787,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8812,21 +8812,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:42</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8842,16 +8842,16 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8862,21 +8862,21 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8892,16 +8892,16 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8912,21 +8912,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>21:09</t>
+          <t>20:48</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8937,21 +8937,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8962,23 +8962,273 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>68</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>105</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
           <t>19:35:56</t>
         </is>
       </c>
-      <c r="B345" t="inlineStr">
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>82</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>21:06</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>115</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>79</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>19:35:56</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>21:09</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>94</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>21:10</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>82</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>19:35:56</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>113</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>19:35:56</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
         <is>
           <t>21:33</t>
         </is>
       </c>
-      <c r="C345" t="inlineStr">
+      <c r="C353" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D345" t="n">
+      <c r="D353" t="n">
         <v>118</v>
       </c>
-      <c r="E345" t="inlineStr">
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>106</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>118</v>
+      </c>
+      <c r="E355" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9013,7 +9263,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:35:56</t>
+          <t>Última actualización: 19:48:11</t>
         </is>
       </c>
     </row>
@@ -10412,7 +10662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10430,14 +10680,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:35:56</t>
+          <t>Última actualización: 19:48:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -11513,6 +11763,31 @@
         <v>100</v>
       </c>
       <c r="E47" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>64</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 181
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E355"/>
+  <dimension ref="A1:E358"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:48:11</t>
+          <t>Última actualización: 19:55:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 350</t>
+          <t>Total filas: 353</t>
         </is>
       </c>
     </row>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4337,7 +4337,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4347,11 +4347,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4372,11 +4372,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -6822,7 +6822,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D259" t="n">
@@ -6837,7 +6837,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>16:44:12</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -6847,11 +6847,11 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6862,7 +6862,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>16:44:12</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6872,11 +6872,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -7887,7 +7887,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7897,11 +7897,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7937,7 +7937,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -7947,11 +7947,11 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -8487,12 +8487,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>20:07</t>
+          <t>20:06</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -8501,7 +8501,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8512,7 +8512,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8522,11 +8522,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8542,16 +8542,16 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>20:08</t>
+          <t>20:07</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8562,12 +8562,12 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:08</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -8576,7 +8576,7 @@
         </is>
       </c>
       <c r="D329" t="n">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8592,16 +8592,16 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8612,7 +8612,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8622,11 +8622,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,21 +8637,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8662,21 +8662,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8687,12 +8687,12 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
@@ -8701,7 +8701,7 @@
         </is>
       </c>
       <c r="D334" t="n">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8712,21 +8712,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8737,12 +8737,12 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
@@ -8751,7 +8751,7 @@
         </is>
       </c>
       <c r="D336" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8762,21 +8762,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>20:33</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,12 +8787,12 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>20:34</t>
+          <t>20:33</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
@@ -8801,7 +8801,7 @@
         </is>
       </c>
       <c r="D338" t="n">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8812,21 +8812,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>20:42</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8837,12 +8837,12 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:42</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
@@ -8851,7 +8851,7 @@
         </is>
       </c>
       <c r="D340" t="n">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8862,12 +8862,12 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
@@ -8876,7 +8876,7 @@
         </is>
       </c>
       <c r="D341" t="n">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8887,21 +8887,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8912,12 +8912,12 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
@@ -8926,7 +8926,7 @@
         </is>
       </c>
       <c r="D343" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8937,21 +8937,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:48</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8967,16 +8967,16 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8987,21 +8987,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9012,12 +9012,12 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
@@ -9026,7 +9026,7 @@
         </is>
       </c>
       <c r="D347" t="n">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9042,16 +9042,16 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9062,21 +9062,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9087,21 +9087,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>21:09</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9117,16 +9117,16 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9142,16 +9142,16 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:09</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9162,21 +9162,21 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9187,21 +9187,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9212,23 +9212,98 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D355" t="n">
         <v>118</v>
       </c>
       <c r="E355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>106</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>19:55:23</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>99</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>118</v>
+      </c>
+      <c r="E358" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9263,7 +9338,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:48:11</t>
+          <t>Última actualización: 19:55:23</t>
         </is>
       </c>
     </row>
@@ -10680,7 +10755,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:48:11</t>
+          <t>Última actualización: 19:55:23</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 182
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E358"/>
+  <dimension ref="A1:E361"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:55:23</t>
+          <t>Última actualización: 20:12:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 353</t>
+          <t>Total filas: 356</t>
         </is>
       </c>
     </row>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -4337,7 +4337,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4347,11 +4347,11 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4372,11 +4372,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -5737,7 +5737,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>14:12:26</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -5747,11 +5747,11 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,7 +5762,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>14:12:26</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -5772,11 +5772,11 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -6812,7 +6812,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>17:48:33</t>
+          <t>16:44:12</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -6822,11 +6822,11 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6862,7 +6862,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>16:44:12</t>
+          <t>17:48:33</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6872,11 +6872,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -7412,7 +7412,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7422,11 +7422,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7437,7 +7437,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7447,11 +7447,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7972,7 +7972,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -7997,7 +7997,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -8512,7 +8512,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8522,11 +8522,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,7 +8537,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8547,11 +8547,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -9087,21 +9087,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>20:12:03</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9112,12 +9112,12 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
@@ -9126,7 +9126,7 @@
         </is>
       </c>
       <c r="D351" t="n">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9137,21 +9137,21 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>21:09</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9162,12 +9162,12 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:09</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
@@ -9176,7 +9176,7 @@
         </is>
       </c>
       <c r="D353" t="n">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9187,21 +9187,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9217,16 +9217,16 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9237,12 +9237,12 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
@@ -9251,7 +9251,7 @@
         </is>
       </c>
       <c r="D356" t="n">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9262,7 +9262,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>19:55:23</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -9272,11 +9272,11 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9287,23 +9287,98 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
+          <t>19:55:23</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>99</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>20:12:03</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>86</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
           <t>19:48:11</t>
         </is>
       </c>
-      <c r="B358" t="inlineStr">
+      <c r="B360" t="inlineStr">
         <is>
           <t>21:46</t>
         </is>
       </c>
-      <c r="C358" t="inlineStr">
+      <c r="C360" t="inlineStr">
         <is>
           <t>14X44_ABASTO</t>
         </is>
       </c>
-      <c r="D358" t="n">
+      <c r="D360" t="n">
         <v>118</v>
       </c>
-      <c r="E358" t="inlineStr">
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>20:12:03</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>95</v>
+      </c>
+      <c r="E361" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9338,7 +9413,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:55:23</t>
+          <t>Última actualización: 20:12:03</t>
         </is>
       </c>
     </row>
@@ -10737,7 +10812,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10755,14 +10830,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:55:23</t>
+          <t>Última actualización: 20:12:03</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 44</t>
         </is>
       </c>
     </row>
@@ -11863,6 +11938,31 @@
         <v>64</v>
       </c>
       <c r="E48" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>20:12:03</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>78</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 183
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E361"/>
+  <dimension ref="A1:E365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:03</t>
+          <t>Última actualización: 20:32:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 356</t>
+          <t>Total filas: 360</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,7 +3012,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3022,11 +3022,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -6362,7 +6362,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>16:28:03</t>
+          <t>15:17:33</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -6372,11 +6372,11 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,7 +6387,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>15:17:33</t>
+          <t>16:28:03</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -6397,11 +6397,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>110</v>
+        <v>39</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7762,7 +7762,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7772,11 +7772,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7787,7 +7787,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -7797,11 +7797,11 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8362,7 +8362,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -8372,11 +8372,11 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8612,7 +8612,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:31:25</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8622,11 +8622,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,7 +8637,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>18:31:25</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8647,11 +8647,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8837,21 +8837,21 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>20:32:13</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>20:42</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8862,12 +8862,12 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>20:43</t>
+          <t>20:42</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
@@ -8876,7 +8876,7 @@
         </is>
       </c>
       <c r="D341" t="n">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8887,12 +8887,12 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>20:46</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
@@ -8901,7 +8901,7 @@
         </is>
       </c>
       <c r="D342" t="n">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8912,21 +8912,21 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8937,12 +8937,12 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>18:52:02</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>20:48</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -8951,7 +8951,7 @@
         </is>
       </c>
       <c r="D344" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8962,21 +8962,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>18:52:02</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:48</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8987,7 +8987,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>19:55:23</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -8997,11 +8997,11 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9012,12 +9012,12 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
@@ -9026,7 +9026,7 @@
         </is>
       </c>
       <c r="D347" t="n">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9037,7 +9037,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -9047,11 +9047,11 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9062,21 +9062,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9087,7 +9087,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>20:12:03</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -9097,11 +9097,11 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9112,21 +9112,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>19:11:45</t>
+          <t>20:12:03</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>21:06</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9137,12 +9137,12 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:11:45</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:06</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
@@ -9151,7 +9151,7 @@
         </is>
       </c>
       <c r="D352" t="n">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9162,21 +9162,21 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>21:09</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9187,12 +9187,12 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>21:10</t>
+          <t>21:09</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
@@ -9201,7 +9201,7 @@
         </is>
       </c>
       <c r="D354" t="n">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9212,21 +9212,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>19:35:56</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>21:10</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9242,16 +9242,16 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9262,12 +9262,12 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:35:56</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
@@ -9276,7 +9276,7 @@
         </is>
       </c>
       <c r="D357" t="n">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9287,7 +9287,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>19:55:23</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -9297,11 +9297,11 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9312,12 +9312,12 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>20:12:03</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:34</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
@@ -9326,7 +9326,7 @@
         </is>
       </c>
       <c r="D359" t="n">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9337,21 +9337,21 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>20:12:03</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9362,23 +9362,123 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
+          <t>19:48:11</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>118</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
           <t>20:12:03</t>
         </is>
       </c>
-      <c r="B361" t="inlineStr">
+      <c r="B362" t="inlineStr">
         <is>
           <t>21:47</t>
         </is>
       </c>
-      <c r="C361" t="inlineStr">
+      <c r="C362" t="inlineStr">
         <is>
           <t>23_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D361" t="n">
+      <c r="D362" t="n">
         <v>95</v>
       </c>
-      <c r="E361" t="inlineStr">
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>20:32:13</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>21:49</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>77</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>20:32:13</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>92</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>20:32:13</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>22:11</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>99</v>
+      </c>
+      <c r="E365" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9413,7 +9513,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:03</t>
+          <t>Última actualización: 20:32:13</t>
         </is>
       </c>
     </row>
@@ -10812,7 +10912,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10830,14 +10930,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:03</t>
+          <t>Última actualización: 20:32:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 44</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -11965,6 +12065,31 @@
       <c r="E49" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>20:32:13</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>108</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 184
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E365"/>
+  <dimension ref="A1:E369"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:32:13</t>
+          <t>Última actualización: 20:46:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 360</t>
+          <t>Total filas: 364</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>11:52:01</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3772,11 +3772,11 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:52:01</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D210" t="n">
@@ -5612,7 +5612,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5622,11 +5622,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -8987,7 +8987,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -8997,11 +8997,11 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9012,7 +9012,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>19:55:23</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -9022,11 +9022,11 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9287,7 +9287,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -9297,11 +9297,11 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9312,7 +9312,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>19:55:23</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -9322,11 +9322,11 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9437,21 +9437,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>20:32:13</t>
+          <t>20:46:10</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>21:50</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9467,18 +9467,118 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>92</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>20:32:13</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
           <t>22:11</t>
         </is>
       </c>
-      <c r="C365" t="inlineStr">
+      <c r="C366" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D365" t="n">
+      <c r="D366" t="n">
         <v>99</v>
       </c>
-      <c r="E365" t="inlineStr">
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>20:46:10</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>108</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>20:46:10</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>108</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>20:46:10</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>22:44</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>118</v>
+      </c>
+      <c r="E369" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9495,7 +9595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9513,14 +9613,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:32:13</t>
+          <t>Última actualización: 20:46:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 54</t>
+          <t>Total filas: 55</t>
         </is>
       </c>
     </row>
@@ -10589,7 +10689,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -10614,7 +10714,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -10896,6 +10996,31 @@
         <v>116</v>
       </c>
       <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>20:46:10</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>108</v>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10912,7 +11037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10930,14 +11055,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:32:13</t>
+          <t>Última actualización: 20:46:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -12046,12 +12171,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20:12:03</t>
+          <t>20:46:10</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -12060,7 +12185,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -12071,23 +12196,48 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>20:12:03</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>78</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>20:32:13</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D50" t="n">
+      <c r="D51" t="n">
         <v>108</v>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 185
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E369"/>
+  <dimension ref="A1:E373"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:46:11</t>
+          <t>Última actualización: 20:52:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 364</t>
+          <t>Total filas: 368</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>10:05:51</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>107</v>
+        <v>5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:05:51</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3047,11 +3047,11 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>5</v>
+        <v>107</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3587,7 +3587,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -5037,7 +5037,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>13:41:54</t>
+          <t>12:52:52</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5047,11 +5047,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5062,7 +5062,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>12:52:52</t>
+          <t>13:41:54</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -5072,11 +5072,11 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>14:53:07</t>
+          <t>13:56:11</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D210" t="n">
@@ -5612,7 +5612,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>13:56:11</t>
+          <t>14:53:07</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -5622,11 +5622,11 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -6437,7 +6437,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>15:46:07</t>
+          <t>16:14:44</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6447,11 +6447,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6462,7 +6462,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>16:14:44</t>
+          <t>15:46:07</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -6472,11 +6472,11 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -7887,7 +7887,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7897,11 +7897,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7937,7 +7937,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -7947,11 +7947,11 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -8462,7 +8462,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -8472,11 +8472,11 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8487,7 +8487,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>19:55:23</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -8497,11 +8497,11 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8987,7 +8987,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>19:55:23</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -8997,11 +8997,11 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9012,7 +9012,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>19:55:23</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -9022,11 +9022,11 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9362,12 +9362,12 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>19:48:11</t>
+          <t>20:52:41</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
@@ -9376,7 +9376,7 @@
         </is>
       </c>
       <c r="D361" t="n">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9387,21 +9387,21 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>20:12:03</t>
+          <t>19:48:11</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9412,12 +9412,12 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>20:32:13</t>
+          <t>20:12:03</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>21:49</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
@@ -9426,7 +9426,7 @@
         </is>
       </c>
       <c r="D363" t="n">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9437,12 +9437,12 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>20:46:10</t>
+          <t>20:32:13</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>21:50</t>
+          <t>21:49</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
@@ -9451,7 +9451,7 @@
         </is>
       </c>
       <c r="D364" t="n">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9462,21 +9462,21 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>20:32:13</t>
+          <t>20:46:10</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>21:50</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9487,21 +9487,21 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>20:32:13</t>
+          <t>20:52:41</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>22:11</t>
+          <t>21:51</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9512,21 +9512,21 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>20:46:10</t>
+          <t>20:32:13</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9537,21 +9537,21 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>20:46:10</t>
+          <t>20:32:13</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:11</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9562,23 +9562,123 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
+          <t>20:52:41</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>101</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
           <t>20:46:10</t>
         </is>
       </c>
-      <c r="B369" t="inlineStr">
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>108</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>20:46:10</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>108</v>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>20:52:41</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>22:43</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>111</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>20:46:10</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
         <is>
           <t>22:44</t>
         </is>
       </c>
-      <c r="C369" t="inlineStr">
+      <c r="C373" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D369" t="n">
+      <c r="D373" t="n">
         <v>118</v>
       </c>
-      <c r="E369" t="inlineStr">
+      <c r="E373" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9595,7 +9695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9613,14 +9713,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:46:11</t>
+          <t>Última actualización: 20:52:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 55</t>
+          <t>Total filas: 56</t>
         </is>
       </c>
     </row>
@@ -10689,7 +10789,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -10714,7 +10814,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -11004,23 +11104,48 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
+          <t>20:52:41</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>22:33</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>101</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
           <t>20:46:10</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B61" t="inlineStr">
         <is>
           <t>22:34</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D60" t="n">
+      <c r="D61" t="n">
         <v>108</v>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11037,7 +11162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11055,14 +11180,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:46:11</t>
+          <t>Última actualización: 20:52:41</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -12196,12 +12321,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:12:03</t>
+          <t>20:52:41</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:30</t>
+          <t>20:54</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -12210,7 +12335,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -12221,23 +12346,98 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>20:52:41</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>37</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>20:12:03</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>78</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>20:52:41</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>22:19</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>87</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>20:32:13</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B54" t="inlineStr">
         <is>
           <t>22:20</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D54" t="n">
         <v>108</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 186
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-11.xlsx
+++ b/data/horarios-141-2026-01-11.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E373"/>
+  <dimension ref="A1:E379"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:41</t>
+          <t>Última actualización: 22:03:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 368</t>
+          <t>Total filas: 374</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>09:23:23</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>09:23:23</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2522,11 +2522,11 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>10:50:41</t>
+          <t>10:37:52</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3072,11 +3072,11 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>10:37:52</t>
+          <t>10:50:41</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3097,11 +3097,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D120" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -3587,7 +3587,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>11:34:59</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:34:59</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3622,11 +3622,11 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>11:47:17</t>
+          <t>11:11:33</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>11:11:33</t>
+          <t>11:47:17</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -4512,7 +4512,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>12:11:52</t>
+          <t>12:45:56</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4522,11 +4522,11 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>12:45:56</t>
+          <t>12:11:52</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4547,11 +4547,11 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D273" t="n">
@@ -7197,7 +7197,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D274" t="n">
@@ -7412,7 +7412,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>16:37:06</t>
+          <t>17:13:39</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -7422,11 +7422,11 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>15X38_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7437,7 +7437,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>17:13:39</t>
+          <t>16:37:06</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7447,11 +7447,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15X38_ABASTO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7762,7 +7762,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:12:30</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -7772,11 +7772,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7787,7 +7787,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>18:12:30</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -7797,11 +7797,11 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>18:44:57</t>
+          <t>17:56:03</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8362,7 +8362,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>17:56:03</t>
+          <t>18:44:57</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -8372,11 +8372,11 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -9637,21 +9637,21 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>20:52:41</t>
+          <t>22:03:17</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>22:43</t>
+          <t>22:41</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D372" t="n">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9662,23 +9662,173 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
+          <t>20:52:41</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>22:43</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>111</v>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
           <t>20:46:10</t>
         </is>
       </c>
-      <c r="B373" t="inlineStr">
+      <c r="B374" t="inlineStr">
         <is>
           <t>22:44</t>
         </is>
       </c>
-      <c r="C373" t="inlineStr">
+      <c r="C374" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D373" t="n">
+      <c r="D374" t="n">
         <v>118</v>
       </c>
-      <c r="E373" t="inlineStr">
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>22:03:17</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>23:04</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>61</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>22:03:17</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>23:19</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D376" t="n">
+        <v>76</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>22:03:17</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>23:34</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>91</v>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>22:03:17</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>23:40</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D378" t="n">
+        <v>97</v>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>22:03:17</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>23:59</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>116</v>
+      </c>
+      <c r="E379" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9695,7 +9845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9713,14 +9863,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:41</t>
+          <t>Última actualización: 22:03:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 56</t>
+          <t>Total filas: 57</t>
         </is>
       </c>
     </row>
@@ -10789,7 +10939,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -10814,7 +10964,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215_EL PELIGRO</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -11146,6 +11296,31 @@
         <v>108</v>
       </c>
       <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>22:03:17</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>23:40</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>97</v>
+      </c>
+      <c r="E62" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11180,7 +11355,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:52:41</t>
+          <t>Última actualización: 22:03:17</t>
         </is>
       </c>
     </row>

</xml_diff>